<commit_message>
correct and parse bright vs. dark analysis
</commit_message>
<xml_diff>
--- a/CL Brightness DUvsDTh mol%.xlsx
+++ b/CL Brightness DUvsDTh mol%.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Library/CloudStorage/Dropbox/My Mac (KU-C02DG1NKML86)/Documents/GitHub/DUDThZircon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/DUDThZircon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BDFC9F-AE6A-7A40-ABDE-B349898EFEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF48B0-5A3D-5F44-A61E-CF31F7D830DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="36740" windowHeight="26760" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
+    <workbookView xWindow="3820" yWindow="1300" windowWidth="28180" windowHeight="27500" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="275">
   <si>
     <t>DARK</t>
   </si>
@@ -834,34 +834,13 @@
     <t>J085</t>
   </si>
   <si>
-    <t>J086</t>
-  </si>
-  <si>
-    <t>J087</t>
-  </si>
-  <si>
-    <t>J088</t>
-  </si>
-  <si>
     <t>J089</t>
   </si>
   <si>
     <t>J090</t>
   </si>
   <si>
-    <t>J092</t>
-  </si>
-  <si>
-    <t>J093</t>
-  </si>
-  <si>
-    <t>J094</t>
-  </si>
-  <si>
     <t>J095</t>
-  </si>
-  <si>
-    <t>J096</t>
   </si>
   <si>
     <t>J097</t>
@@ -8066,7 +8045,7 @@
   <dimension ref="A1:H272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E270" sqref="E270"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8158,7 +8137,7 @@
         <v>5.0756553725014468</v>
       </c>
       <c r="E4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" t="s">
         <v>100</v>
@@ -8183,7 +8162,7 @@
         <v>3.4259373103493878</v>
       </c>
       <c r="E5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
@@ -8208,7 +8187,7 @@
         <v>2.299376124257801</v>
       </c>
       <c r="E6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F6" t="s">
         <v>100</v>
@@ -8233,7 +8212,7 @@
         <v>3.9349523259227679</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F7" t="s">
         <v>100</v>
@@ -8258,7 +8237,7 @@
         <v>3.2563704123400972</v>
       </c>
       <c r="E8" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F8" t="s">
         <v>100</v>
@@ -8294,7 +8273,7 @@
         <v>1.1839608725724289</v>
       </c>
       <c r="E10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -8319,7 +8298,7 @@
         <v>1.3369696674615874</v>
       </c>
       <c r="E11" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
@@ -8344,7 +8323,7 @@
         <v>1.5179302831953077</v>
       </c>
       <c r="E12" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -8369,7 +8348,7 @@
         <v>1.185623697515116</v>
       </c>
       <c r="E13" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
@@ -8394,7 +8373,7 @@
         <v>0.62932227134606444</v>
       </c>
       <c r="E14" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -8419,7 +8398,7 @@
         <v>1.281962388060818</v>
       </c>
       <c r="E15" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -8444,7 +8423,7 @@
         <v>0.59474135948255069</v>
       </c>
       <c r="E16" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -8480,17 +8459,17 @@
         <v>0.30806295223046032</v>
       </c>
       <c r="E18" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F18" t="s">
         <v>100</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G17:G80" si="2">B18</f>
+        <f t="shared" ref="G18:G80" si="2">B18</f>
         <v>0.85176930936848871</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H17:H80" si="3">C18</f>
+        <f t="shared" ref="H18:H80" si="3">C18</f>
         <v>0.30806295223046032</v>
       </c>
     </row>
@@ -8505,7 +8484,7 @@
         <v>4.3317023123668212</v>
       </c>
       <c r="E19" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F19" t="s">
         <v>100</v>
@@ -8530,7 +8509,7 @@
         <v>3.7223581406360982</v>
       </c>
       <c r="E20" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F20" t="s">
         <v>100</v>
@@ -8555,7 +8534,7 @@
         <v>1.6304705475252395</v>
       </c>
       <c r="E21" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F21" t="s">
         <v>100</v>
@@ -8580,7 +8559,7 @@
         <v>3.228177000176053</v>
       </c>
       <c r="E22" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F22" t="s">
         <v>100</v>
@@ -8610,7 +8589,7 @@
         <v>2.2657963741897467</v>
       </c>
       <c r="E24" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F24" t="s">
         <v>19</v>
@@ -8635,7 +8614,7 @@
         <v>1.9294507158677578</v>
       </c>
       <c r="E25" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -8660,7 +8639,7 @@
         <v>3.6293152423273187</v>
       </c>
       <c r="E26" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F26" t="s">
         <v>19</v>
@@ -8685,7 +8664,7 @@
         <v>1.9948720122277863</v>
       </c>
       <c r="E27" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -8710,7 +8689,7 @@
         <v>5.9811481138602263</v>
       </c>
       <c r="E28" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -8735,7 +8714,7 @@
         <v>6.30230907131146</v>
       </c>
       <c r="E29" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
@@ -8760,7 +8739,7 @@
         <v>3.1716406940184645</v>
       </c>
       <c r="E30" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
@@ -8785,7 +8764,7 @@
         <v>4.6206567284736986</v>
       </c>
       <c r="E31" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
@@ -8810,7 +8789,7 @@
         <v>3.7862290014209905</v>
       </c>
       <c r="E32" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F32" t="s">
         <v>19</v>
@@ -8835,7 +8814,7 @@
         <v>4.8235911796475524</v>
       </c>
       <c r="E33" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -8860,7 +8839,7 @@
         <v>4.5088139200237221</v>
       </c>
       <c r="E34" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -8885,7 +8864,7 @@
         <v>3.4054873792273064</v>
       </c>
       <c r="E35" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F35" t="s">
         <v>19</v>
@@ -8910,7 +8889,7 @@
         <v>2.2428135785454968</v>
       </c>
       <c r="E36" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -8935,7 +8914,7 @@
         <v>4.2449061314374834</v>
       </c>
       <c r="E37" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -8960,7 +8939,7 @@
         <v>1.8681908415946771</v>
       </c>
       <c r="E38" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -8985,7 +8964,7 @@
         <v>1.5504938593881847</v>
       </c>
       <c r="E39" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F39" t="s">
         <v>19</v>
@@ -9010,7 +8989,7 @@
         <v>1.4696247639977418</v>
       </c>
       <c r="E40" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F40" t="s">
         <v>19</v>
@@ -9035,7 +9014,7 @@
         <v>0.69340043588327072</v>
       </c>
       <c r="E41" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F41" t="s">
         <v>19</v>
@@ -9071,7 +9050,7 @@
         <v>2.2314273473202855</v>
       </c>
       <c r="E43" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F43" t="s">
         <v>100</v>
@@ -9096,7 +9075,7 @@
         <v>2.4477768915032745</v>
       </c>
       <c r="E44" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F44" t="s">
         <v>100</v>
@@ -9121,7 +9100,7 @@
         <v>2.3563675232249914</v>
       </c>
       <c r="E45" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F45" t="s">
         <v>100</v>
@@ -9146,7 +9125,7 @@
         <v>3.5267092538532787</v>
       </c>
       <c r="E46" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F46" t="s">
         <v>100</v>
@@ -9171,7 +9150,7 @@
         <v>2.9833949280009415</v>
       </c>
       <c r="E47" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F47" t="s">
         <v>100</v>
@@ -9196,7 +9175,7 @@
         <v>4.2868052473220164</v>
       </c>
       <c r="E48" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F48" t="s">
         <v>100</v>
@@ -9221,7 +9200,7 @@
         <v>2.6776305772606701</v>
       </c>
       <c r="E49" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F49" t="s">
         <v>100</v>
@@ -9246,7 +9225,7 @@
         <v>2.1088591124519684</v>
       </c>
       <c r="E50" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F50" t="s">
         <v>100</v>
@@ -9271,7 +9250,7 @@
         <v>1.2161698517581965</v>
       </c>
       <c r="E51" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F51" t="s">
         <v>100</v>
@@ -9301,7 +9280,7 @@
         <v>1.2367244794448276</v>
       </c>
       <c r="E53" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F53" t="s">
         <v>19</v>
@@ -9326,7 +9305,7 @@
         <v>1.2219422663406996</v>
       </c>
       <c r="E54" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F54" t="s">
         <v>19</v>
@@ -9351,7 +9330,7 @@
         <v>1.4440836442525344</v>
       </c>
       <c r="E55" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F55" t="s">
         <v>19</v>
@@ -9376,7 +9355,7 @@
         <v>1.2619554546141456</v>
       </c>
       <c r="E56" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F56" t="s">
         <v>19</v>
@@ -9401,7 +9380,7 @@
         <v>1.5056618667346613</v>
       </c>
       <c r="E57" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F57" t="s">
         <v>19</v>
@@ -9426,7 +9405,7 @@
         <v>0.6680256881830372</v>
       </c>
       <c r="E58" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F58" t="s">
         <v>19</v>
@@ -9451,7 +9430,7 @@
         <v>0.69458815039000721</v>
       </c>
       <c r="E59" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F59" t="s">
         <v>19</v>
@@ -9476,7 +9455,7 @@
         <v>1.4156301158353326</v>
       </c>
       <c r="E60" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F60" t="s">
         <v>19</v>
@@ -9501,7 +9480,7 @@
         <v>1.3570013229388698</v>
       </c>
       <c r="E61" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F61" t="s">
         <v>19</v>
@@ -9550,7 +9529,7 @@
         <v>4.1537697297805343</v>
       </c>
       <c r="E64" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F64" t="s">
         <v>100</v>
@@ -9575,7 +9554,7 @@
         <v>3.7858119230342955</v>
       </c>
       <c r="E65" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F65" t="s">
         <v>100</v>
@@ -9600,7 +9579,7 @@
         <v>3.7773257279032615</v>
       </c>
       <c r="E66" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F66" t="s">
         <v>100</v>
@@ -9625,7 +9604,7 @@
         <v>3.7659889713096049</v>
       </c>
       <c r="E67" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F67" t="s">
         <v>100</v>
@@ -9650,7 +9629,7 @@
         <v>4.8782065855686172</v>
       </c>
       <c r="E68" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F68" t="s">
         <v>100</v>
@@ -9675,7 +9654,7 @@
         <v>6.0123363209671385</v>
       </c>
       <c r="E69" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F69" t="s">
         <v>100</v>
@@ -9700,7 +9679,7 @@
         <v>5.7641351612977143</v>
       </c>
       <c r="E70" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F70" t="s">
         <v>100</v>
@@ -9725,7 +9704,7 @@
         <v>5.2110866742621136</v>
       </c>
       <c r="E71" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F71" t="s">
         <v>100</v>
@@ -9750,7 +9729,7 @@
         <v>4.0348660948858344</v>
       </c>
       <c r="E72" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F72" t="s">
         <v>100</v>
@@ -9775,7 +9754,7 @@
         <v>5.9284951481007964</v>
       </c>
       <c r="E73" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F73" t="s">
         <v>100</v>
@@ -9805,7 +9784,7 @@
         <v>1.9921534562762022</v>
       </c>
       <c r="E75" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F75" t="s">
         <v>19</v>
@@ -9830,7 +9809,7 @@
         <v>1.4518278025574454</v>
       </c>
       <c r="E76" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
@@ -9855,7 +9834,7 @@
         <v>1.4729731152108785</v>
       </c>
       <c r="E77" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F77" t="s">
         <v>19</v>
@@ -9880,7 +9859,7 @@
         <v>2.342758012519143</v>
       </c>
       <c r="E78" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -9905,7 +9884,7 @@
         <v>2.3406227425078283</v>
       </c>
       <c r="E79" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -9930,7 +9909,7 @@
         <v>1.789145221273422</v>
       </c>
       <c r="E80" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
@@ -9955,7 +9934,7 @@
         <v>2.1751718942301173</v>
       </c>
       <c r="E81" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F81" t="s">
         <v>19</v>
@@ -9980,7 +9959,7 @@
         <v>1.9971824315645965</v>
       </c>
       <c r="E82" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F82" t="s">
         <v>19</v>
@@ -10005,7 +9984,7 @@
         <v>2.1026664425429034</v>
       </c>
       <c r="E83" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F83" t="s">
         <v>19</v>
@@ -10030,7 +10009,7 @@
         <v>2.5164625065594608</v>
       </c>
       <c r="E84" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F84" t="s">
         <v>19</v>
@@ -10055,7 +10034,7 @@
         <v>1.1669475185950324</v>
       </c>
       <c r="E85" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F85" t="s">
         <v>19</v>
@@ -10080,7 +10059,7 @@
         <v>1.2542826533132139</v>
       </c>
       <c r="E86" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
@@ -10105,7 +10084,7 @@
         <v>2.6443764590992807</v>
       </c>
       <c r="E87" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F87" t="s">
         <v>19</v>
@@ -10130,7 +10109,7 @@
         <v>1.6769207986168109</v>
       </c>
       <c r="E88" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F88" t="s">
         <v>19</v>
@@ -10155,7 +10134,7 @@
         <v>1.7381531037324824</v>
       </c>
       <c r="E89" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F89" t="s">
         <v>19</v>
@@ -10180,7 +10159,7 @@
         <v>0.92069190718101768</v>
       </c>
       <c r="E90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F90" t="s">
         <v>19</v>
@@ -10205,7 +10184,7 @@
         <v>1.6282012179262877</v>
       </c>
       <c r="E91" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F91" t="s">
         <v>19</v>
@@ -10230,7 +10209,7 @@
         <v>2.564635627719027</v>
       </c>
       <c r="E92" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F92" t="s">
         <v>19</v>
@@ -10255,7 +10234,7 @@
         <v>2.7536534919885556</v>
       </c>
       <c r="E93" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F93" t="s">
         <v>19</v>
@@ -10291,7 +10270,7 @@
         <v>4.6312342664074491</v>
       </c>
       <c r="E95" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F95" t="s">
         <v>100</v>
@@ -10316,7 +10295,7 @@
         <v>4.2805447025835299</v>
       </c>
       <c r="E96" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F96" t="s">
         <v>100</v>
@@ -10346,7 +10325,7 @@
         <v>1.8485782405591205</v>
       </c>
       <c r="E98" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F98" t="s">
         <v>19</v>
@@ -10371,7 +10350,7 @@
         <v>1.9219425621635235</v>
       </c>
       <c r="E99" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F99" t="s">
         <v>19</v>
@@ -10396,7 +10375,7 @@
         <v>2.9138606164745458</v>
       </c>
       <c r="E100" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="F100" t="s">
         <v>19</v>
@@ -10432,7 +10411,7 @@
         <v>3.6637499999999998</v>
       </c>
       <c r="E102" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F102" t="s">
         <v>100</v>
@@ -10457,7 +10436,7 @@
         <v>1.8675299999999999</v>
       </c>
       <c r="E103" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F103" t="s">
         <v>100</v>
@@ -10482,7 +10461,7 @@
         <v>5.4247500000000004</v>
       </c>
       <c r="E104" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F104" t="s">
         <v>100</v>
@@ -10507,7 +10486,7 @@
         <v>5.7273199999999997</v>
       </c>
       <c r="E105" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F105" t="s">
         <v>100</v>
@@ -10537,7 +10516,7 @@
         <v>0.38237331951487913</v>
       </c>
       <c r="E107" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F107" t="s">
         <v>19</v>
@@ -10562,7 +10541,7 @@
         <v>0.57688747081530833</v>
       </c>
       <c r="E108" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F108" t="s">
         <v>19</v>
@@ -10587,7 +10566,7 @@
         <v>0.68603967371369023</v>
       </c>
       <c r="E109" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F109" t="s">
         <v>19</v>
@@ -10612,7 +10591,7 @@
         <v>0.89737468777474383</v>
       </c>
       <c r="E110" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
@@ -10653,7 +10632,7 @@
         <v>0.84843729771696497</v>
       </c>
       <c r="E113" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F113" t="s">
         <v>100</v>
@@ -10678,7 +10657,7 @@
         <v>1.4562974982687191</v>
       </c>
       <c r="E114" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F114" t="s">
         <v>100</v>
@@ -10703,7 +10682,7 @@
         <v>1.069642209397383</v>
       </c>
       <c r="E115" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F115" t="s">
         <v>100</v>
@@ -10728,7 +10707,7 @@
         <v>1.1791230948075282</v>
       </c>
       <c r="E116" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F116" t="s">
         <v>100</v>
@@ -10753,7 +10732,7 @@
         <v>0.63699997333663083</v>
       </c>
       <c r="E117" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F117" t="s">
         <v>100</v>
@@ -10778,7 +10757,7 @@
         <v>1.3258939635839924</v>
       </c>
       <c r="E118" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F118" t="s">
         <v>100</v>
@@ -10803,7 +10782,7 @@
         <v>0.72744043320347707</v>
       </c>
       <c r="E119" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F119" t="s">
         <v>100</v>
@@ -10828,7 +10807,7 @@
         <v>0.7281358184247112</v>
       </c>
       <c r="E120" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F120" t="s">
         <v>100</v>
@@ -10853,7 +10832,7 @@
         <v>0.80594501647977168</v>
       </c>
       <c r="E121" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F121" t="s">
         <v>100</v>
@@ -10878,7 +10857,7 @@
         <v>1.0296207117444911</v>
       </c>
       <c r="E122" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F122" t="s">
         <v>100</v>
@@ -10908,7 +10887,7 @@
         <v>0.51823237441750658</v>
       </c>
       <c r="E124" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F124" t="s">
         <v>19</v>
@@ -10933,7 +10912,7 @@
         <v>0.63363229466700532</v>
       </c>
       <c r="E125" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F125" t="s">
         <v>19</v>
@@ -10958,7 +10937,7 @@
         <v>0.66471932407842638</v>
       </c>
       <c r="E126" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F126" t="s">
         <v>19</v>
@@ -10983,7 +10962,7 @@
         <v>0.83264781158263135</v>
       </c>
       <c r="E127" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F127" t="s">
         <v>19</v>
@@ -11008,7 +10987,7 @@
         <v>0.75321928382382142</v>
       </c>
       <c r="E128" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F128" t="s">
         <v>19</v>
@@ -11033,7 +11012,7 @@
         <v>1.1767588988982671</v>
       </c>
       <c r="E129" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F129" t="s">
         <v>19</v>
@@ -11058,7 +11037,7 @@
         <v>0.64122351712986858</v>
       </c>
       <c r="E130" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F130" t="s">
         <v>19</v>
@@ -11083,7 +11062,7 @@
         <v>0.56078467475847971</v>
       </c>
       <c r="E131" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F131" t="s">
         <v>19</v>
@@ -11108,7 +11087,7 @@
         <v>0.52603573495381228</v>
       </c>
       <c r="E132" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F132" t="s">
         <v>19</v>
@@ -11133,7 +11112,7 @@
         <v>0.55511474815927786</v>
       </c>
       <c r="E133" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F133" t="s">
         <v>19</v>
@@ -11158,7 +11137,7 @@
         <v>0.42559382391712486</v>
       </c>
       <c r="E134" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F134" t="s">
         <v>19</v>
@@ -11183,7 +11162,7 @@
         <v>0.72964321318336167</v>
       </c>
       <c r="E135" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F135" t="s">
         <v>19</v>
@@ -11208,7 +11187,7 @@
         <v>0.73294690773396087</v>
       </c>
       <c r="E136" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F136" t="s">
         <v>19</v>
@@ -11233,7 +11212,7 @@
         <v>0.72479245056849606</v>
       </c>
       <c r="E137" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F137" t="s">
         <v>19</v>
@@ -11258,7 +11237,7 @@
         <v>1.6352156002086744E-2</v>
       </c>
       <c r="E138" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F138" t="s">
         <v>19</v>
@@ -11283,7 +11262,7 @@
         <v>6.8053032074691044E-2</v>
       </c>
       <c r="E139" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F139" t="s">
         <v>19</v>
@@ -11319,7 +11298,7 @@
         <v>3.805179678278277</v>
       </c>
       <c r="E141" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F141" t="s">
         <v>100</v>
@@ -11344,7 +11323,7 @@
         <v>4.408703132775754</v>
       </c>
       <c r="E142" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F142" t="s">
         <v>100</v>
@@ -11369,7 +11348,7 @@
         <v>2.8162804046730301</v>
       </c>
       <c r="E143" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F143" t="s">
         <v>100</v>
@@ -11394,7 +11373,7 @@
         <v>3.9858855422053012</v>
       </c>
       <c r="E144" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F144" t="s">
         <v>100</v>
@@ -11419,7 +11398,7 @@
         <v>2.0046639674564561</v>
       </c>
       <c r="E145" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F145" t="s">
         <v>100</v>
@@ -11444,7 +11423,7 @@
         <v>7.206036327453651</v>
       </c>
       <c r="E146" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F146" t="s">
         <v>100</v>
@@ -11469,7 +11448,7 @@
         <v>7.183874727453067</v>
       </c>
       <c r="E147" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F147" t="s">
         <v>100</v>
@@ -11494,7 +11473,7 @@
         <v>2.0247524752475243</v>
       </c>
       <c r="E148" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F148" t="s">
         <v>100</v>
@@ -11519,7 +11498,7 @@
         <v>1.0720407861681689</v>
       </c>
       <c r="E149" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F149" t="s">
         <v>100</v>
@@ -11544,7 +11523,7 @@
         <v>0.77774493867297168</v>
       </c>
       <c r="E150" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F150" t="s">
         <v>100</v>
@@ -11569,7 +11548,7 @@
         <v>1.540121176296734</v>
       </c>
       <c r="E151" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F151" t="s">
         <v>100</v>
@@ -11594,7 +11573,7 @@
         <v>0.4838924190926554</v>
       </c>
       <c r="E152" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F152" t="s">
         <v>100</v>
@@ -11619,7 +11598,7 @@
         <v>0.70769912812176727</v>
       </c>
       <c r="E153" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F153" t="s">
         <v>100</v>
@@ -11649,7 +11628,7 @@
         <v>1.4305494406878836</v>
       </c>
       <c r="E155" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F155" t="s">
         <v>19</v>
@@ -11674,7 +11653,7 @@
         <v>0.75540004015422646</v>
       </c>
       <c r="E156" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F156" t="s">
         <v>19</v>
@@ -11699,7 +11678,7 @@
         <v>0.95079060144820415</v>
       </c>
       <c r="E157" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F157" t="s">
         <v>19</v>
@@ -11724,7 +11703,7 @@
         <v>2.229126644007684</v>
       </c>
       <c r="E158" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F158" t="s">
         <v>19</v>
@@ -11749,7 +11728,7 @@
         <v>2.0920644303236289</v>
       </c>
       <c r="E159" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F159" t="s">
         <v>19</v>
@@ -11774,7 +11753,7 @@
         <v>0.66225801684646068</v>
       </c>
       <c r="E160" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F160" t="s">
         <v>19</v>
@@ -11810,7 +11789,7 @@
         <v>1.6293214183937692</v>
       </c>
       <c r="E162" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F162" t="s">
         <v>19</v>
@@ -11835,7 +11814,7 @@
         <v>1.5620599283848617</v>
       </c>
       <c r="E163" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F163" t="s">
         <v>19</v>
@@ -11860,7 +11839,7 @@
         <v>1.1415920316606596</v>
       </c>
       <c r="E164" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F164" t="s">
         <v>19</v>
@@ -11885,7 +11864,7 @@
         <v>0.95630689055293971</v>
       </c>
       <c r="E165" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F165" t="s">
         <v>19</v>
@@ -11910,7 +11889,7 @@
         <v>1.3033671888455811</v>
       </c>
       <c r="E166" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F166" t="s">
         <v>19</v>
@@ -11935,7 +11914,7 @@
         <v>1.0089096012225738</v>
       </c>
       <c r="E167" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F167" t="s">
         <v>19</v>
@@ -11960,7 +11939,7 @@
         <v>0.64456332937641847</v>
       </c>
       <c r="E168" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F168" t="s">
         <v>19</v>
@@ -11985,7 +11964,7 @@
         <v>1.1280540447423508</v>
       </c>
       <c r="E169" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F169" t="s">
         <v>19</v>
@@ -12010,7 +11989,7 @@
         <v>1.276052090514102</v>
       </c>
       <c r="E170" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F170" t="s">
         <v>19</v>
@@ -12035,7 +12014,7 @@
         <v>1.330110704976569</v>
       </c>
       <c r="E171" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F171" t="s">
         <v>19</v>
@@ -12060,7 +12039,7 @@
         <v>1.0989826968432796</v>
       </c>
       <c r="E172" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F172" t="s">
         <v>19</v>
@@ -12085,7 +12064,7 @@
         <v>0.97322401129316305</v>
       </c>
       <c r="E173" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F173" t="s">
         <v>19</v>
@@ -12110,7 +12089,7 @@
         <v>0.97083903452194464</v>
       </c>
       <c r="E174" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F174" t="s">
         <v>19</v>
@@ -12135,7 +12114,7 @@
         <v>0.89742342354126226</v>
       </c>
       <c r="E175" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F175" t="s">
         <v>19</v>
@@ -12160,7 +12139,7 @@
         <v>1.1364933875324057</v>
       </c>
       <c r="E176" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F176" t="s">
         <v>19</v>
@@ -12185,7 +12164,7 @@
         <v>0.46812532863574308</v>
       </c>
       <c r="E177" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F177" t="s">
         <v>19</v>
@@ -12210,7 +12189,7 @@
         <v>0.95630689055293971</v>
       </c>
       <c r="E178" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F178" t="s">
         <v>19</v>
@@ -12235,7 +12214,7 @@
         <v>0.6837605941472884</v>
       </c>
       <c r="E179" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F179" t="s">
         <v>19</v>
@@ -12260,7 +12239,7 @@
         <v>0.53012048252772936</v>
       </c>
       <c r="E180" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F180" t="s">
         <v>19</v>
@@ -12285,7 +12264,7 @@
         <v>0.59310499880298861</v>
       </c>
       <c r="E181" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F181" t="s">
         <v>19</v>
@@ -12310,7 +12289,7 @@
         <v>0.48240967740857427</v>
       </c>
       <c r="E182" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F182" t="s">
         <v>19</v>
@@ -12335,7 +12314,7 @@
         <v>0.45824666440791362</v>
       </c>
       <c r="E183" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F183" t="s">
         <v>19</v>
@@ -12360,7 +12339,7 @@
         <v>0.42640682429331767</v>
       </c>
       <c r="E184" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F184" t="s">
         <v>19</v>
@@ -12390,7 +12369,7 @@
         <v>1.3920827437358692</v>
       </c>
       <c r="E186" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F186" t="s">
         <v>100</v>
@@ -12415,7 +12394,7 @@
         <v>2.6344470538032265</v>
       </c>
       <c r="E187" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F187" t="s">
         <v>100</v>
@@ -12440,7 +12419,7 @@
         <v>1.2876573659521637</v>
       </c>
       <c r="E188" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F188" t="s">
         <v>100</v>
@@ -12465,7 +12444,7 @@
         <v>2.9463274148742036</v>
       </c>
       <c r="E189" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F189" t="s">
         <v>100</v>
@@ -12490,7 +12469,7 @@
         <v>1.9018095272570115</v>
       </c>
       <c r="E190" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F190" t="s">
         <v>100</v>
@@ -12515,7 +12494,7 @@
         <v>4.0094681904869027</v>
       </c>
       <c r="E191" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F191" t="s">
         <v>100</v>
@@ -12540,7 +12519,7 @@
         <v>1.9458432739560734</v>
       </c>
       <c r="E192" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F192" t="s">
         <v>100</v>
@@ -12565,7 +12544,7 @@
         <v>1.6992265822360058</v>
       </c>
       <c r="E193" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F193" t="s">
         <v>100</v>
@@ -12590,7 +12569,7 @@
         <v>4.9781564054012133</v>
       </c>
       <c r="E194" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F194" t="s">
         <v>100</v>
@@ -12615,7 +12594,7 @@
         <v>2.0363160049914404</v>
       </c>
       <c r="E195" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F195" t="s">
         <v>100</v>
@@ -12640,7 +12619,7 @@
         <v>1.5311194345723143</v>
       </c>
       <c r="E196" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F196" t="s">
         <v>100</v>
@@ -12665,7 +12644,7 @@
         <v>4.4436379592518627</v>
       </c>
       <c r="E197" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F197" t="s">
         <v>100</v>
@@ -12690,7 +12669,7 @@
         <v>6.5106315940233568</v>
       </c>
       <c r="E198" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F198" t="s">
         <v>100</v>
@@ -12715,7 +12694,7 @@
         <v>2.1054257091840332</v>
       </c>
       <c r="E199" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F199" t="s">
         <v>100</v>
@@ -12740,7 +12719,7 @@
         <v>2.89553894691355</v>
       </c>
       <c r="E200" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F200" t="s">
         <v>100</v>
@@ -12765,7 +12744,7 @@
         <v>2.4069171308235857</v>
       </c>
       <c r="E201" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F201" t="s">
         <v>100</v>
@@ -12790,7 +12769,7 @@
         <v>1.7553715061227722</v>
       </c>
       <c r="E202" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F202" t="s">
         <v>100</v>
@@ -12815,7 +12794,7 @@
         <v>2.3839342911860308</v>
       </c>
       <c r="E203" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F203" t="s">
         <v>100</v>
@@ -12840,7 +12819,7 @@
         <v>1.7945396109667138</v>
       </c>
       <c r="E204" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F204" t="s">
         <v>100</v>
@@ -12865,7 +12844,7 @@
         <v>1.6212395523817154</v>
       </c>
       <c r="E205" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F205" t="s">
         <v>100</v>
@@ -12890,7 +12869,7 @@
         <v>3.2259945716254927</v>
       </c>
       <c r="E206" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F206" t="s">
         <v>100</v>
@@ -12915,7 +12894,7 @@
         <v>2.0069326735774244</v>
       </c>
       <c r="E207" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F207" t="s">
         <v>100</v>
@@ -12940,7 +12919,7 @@
         <v>2.143013376678518</v>
       </c>
       <c r="E208" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F208" t="s">
         <v>100</v>
@@ -12965,7 +12944,7 @@
         <v>0.62554306569969165</v>
       </c>
       <c r="E209" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F209" t="s">
         <v>100</v>
@@ -13001,7 +12980,7 @@
         <v>1.0857185123673931</v>
       </c>
       <c r="E212" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F212" t="s">
         <v>19</v>
@@ -13026,7 +13005,7 @@
         <v>0.65377352480922901</v>
       </c>
       <c r="E213" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F213" t="s">
         <v>19</v>
@@ -13051,7 +13030,7 @@
         <v>0.70066379308607007</v>
       </c>
       <c r="E214" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F214" t="s">
         <v>19</v>
@@ -13076,7 +13055,7 @@
         <v>1.3533683779214274</v>
       </c>
       <c r="E215" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F215" t="s">
         <v>19</v>
@@ -13101,7 +13080,7 @@
         <v>0.80089753392428087</v>
       </c>
       <c r="E216" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F216" t="s">
         <v>19</v>
@@ -13126,7 +13105,7 @@
         <v>0.57134640411045745</v>
       </c>
       <c r="E217" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F217" t="s">
         <v>19</v>
@@ -13151,7 +13130,7 @@
         <v>1.3055403788057476</v>
       </c>
       <c r="E218" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F218" t="s">
         <v>19</v>
@@ -13176,7 +13155,7 @@
         <v>1.0028688214512544</v>
       </c>
       <c r="E219" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F219" t="s">
         <v>19</v>
@@ -13201,7 +13180,7 @@
         <v>1.231979445145589</v>
       </c>
       <c r="E220" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F220" t="s">
         <v>19</v>
@@ -13226,7 +13205,7 @@
         <v>1.8126857468550253</v>
       </c>
       <c r="E221" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F221" t="s">
         <v>19</v>
@@ -13251,7 +13230,7 @@
         <v>1.0689700407568743</v>
       </c>
       <c r="E222" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F222" t="s">
         <v>19</v>
@@ -13281,7 +13260,7 @@
         <v>1.1753100485560408</v>
       </c>
       <c r="E224" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F224" t="s">
         <v>100</v>
@@ -13306,7 +13285,7 @@
         <v>1.8628343431388317</v>
       </c>
       <c r="E225" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F225" t="s">
         <v>100</v>
@@ -13331,7 +13310,7 @@
         <v>1.2045903552921469</v>
       </c>
       <c r="E226" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F226" t="s">
         <v>100</v>
@@ -13356,7 +13335,7 @@
         <v>1.319218266035356</v>
       </c>
       <c r="E227" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F227" t="s">
         <v>100</v>
@@ -13381,7 +13360,7 @@
         <v>2.6970677264530059</v>
       </c>
       <c r="E228" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F228" t="s">
         <v>100</v>
@@ -13406,7 +13385,7 @@
         <v>0.78992000766093473</v>
       </c>
       <c r="E229" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F229" t="s">
         <v>100</v>
@@ -13431,7 +13410,7 @@
         <v>1.3883916626658384</v>
       </c>
       <c r="E230" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F230" t="s">
         <v>100</v>
@@ -13456,7 +13435,7 @@
         <v>1.4373497113544722</v>
       </c>
       <c r="E231" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F231" t="s">
         <v>100</v>
@@ -13481,7 +13460,7 @@
         <v>1.1543557351309801</v>
       </c>
       <c r="E232" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F232" t="s">
         <v>100</v>
@@ -13506,7 +13485,7 @@
         <v>1.6285222852443999</v>
       </c>
       <c r="E233" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F233" t="s">
         <v>100</v>
@@ -13531,7 +13510,7 @@
         <v>2.3901841722256312</v>
       </c>
       <c r="E234" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F234" t="s">
         <v>100</v>
@@ -13556,7 +13535,7 @@
         <v>1.6099626707873229</v>
       </c>
       <c r="E235" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F235" t="s">
         <v>100</v>
@@ -13581,7 +13560,7 @@
         <v>2.3303523366219281</v>
       </c>
       <c r="E236" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F236" t="s">
         <v>100</v>
@@ -13606,7 +13585,7 @@
         <v>1.7068942899663897</v>
       </c>
       <c r="E237" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F237" t="s">
         <v>100</v>
@@ -13631,7 +13610,7 @@
         <v>0.53301487784246382</v>
       </c>
       <c r="E238" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F238" t="s">
         <v>100</v>
@@ -13667,7 +13646,7 @@
         <v>13.523716572320904</v>
       </c>
       <c r="E240" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F240" t="s">
         <v>100</v>
@@ -13692,7 +13671,7 @@
         <v>7.4400416422669</v>
       </c>
       <c r="E241" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F241" t="s">
         <v>100</v>
@@ -13717,7 +13696,7 @@
         <v>4.4377643307957566</v>
       </c>
       <c r="E242" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F242" t="s">
         <v>100</v>
@@ -13742,7 +13721,7 @@
         <v>5.9510703363914361</v>
       </c>
       <c r="E243" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F243" t="s">
         <v>100</v>
@@ -13767,7 +13746,7 @@
         <v>10.973583186934738</v>
       </c>
       <c r="E244" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F244" t="s">
         <v>100</v>
@@ -13797,7 +13776,7 @@
         <v>6.0390396252195968</v>
       </c>
       <c r="E246" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F246" t="s">
         <v>19</v>
@@ -13822,7 +13801,7 @@
         <v>4.4197410371527095</v>
       </c>
       <c r="E247" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F247" t="s">
         <v>19</v>
@@ -13847,7 +13826,7 @@
         <v>4.8755937276335475</v>
       </c>
       <c r="E248" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F248" t="s">
         <v>19</v>
@@ -13872,7 +13851,7 @@
         <v>1.3043789446287981</v>
       </c>
       <c r="E249" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F249" t="s">
         <v>19</v>
@@ -13897,7 +13876,7 @@
         <v>3.923417268527555</v>
       </c>
       <c r="E250" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F250" t="s">
         <v>19</v>
@@ -13922,7 +13901,7 @@
         <v>5.0871234302817356</v>
       </c>
       <c r="E251" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F251" t="s">
         <v>19</v>
@@ -13947,7 +13926,7 @@
         <v>4.0234888411737906</v>
       </c>
       <c r="E252" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F252" t="s">
         <v>19</v>
@@ -13972,7 +13951,7 @@
         <v>3.3887045351031295</v>
       </c>
       <c r="E253" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F253" t="s">
         <v>19</v>
@@ -13997,7 +13976,7 @@
         <v>6.4176589238076636</v>
       </c>
       <c r="E254" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F254" t="s">
         <v>19</v>
@@ -14022,7 +14001,7 @@
         <v>1.3374324939813909</v>
       </c>
       <c r="E255" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F255" t="s">
         <v>19</v>
@@ -14047,7 +14026,7 @@
         <v>3.7748714945669848</v>
       </c>
       <c r="E256" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F256" t="s">
         <v>19</v>
@@ -14072,7 +14051,7 @@
         <v>4.5460992907801412</v>
       </c>
       <c r="E257" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F257" t="s">
         <v>19</v>
@@ -14097,7 +14076,7 @@
         <v>3.8806688789120947</v>
       </c>
       <c r="E258" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F258" t="s">
         <v>19</v>
@@ -14122,7 +14101,7 @@
         <v>2.7643307957576937</v>
       </c>
       <c r="E259" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F259" t="s">
         <v>19</v>
@@ -14147,7 +14126,7 @@
         <v>4.8396772724315174</v>
       </c>
       <c r="E260" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F260" t="s">
         <v>19</v>
@@ -14172,7 +14151,7 @@
         <v>3.3006701802329359</v>
       </c>
       <c r="E261" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F261" t="s">
         <v>19</v>
@@ -14197,7 +14176,7 @@
         <v>1.6349795041967594</v>
       </c>
       <c r="E262" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F262" t="s">
         <v>19</v>
@@ -14222,7 +14201,7 @@
         <v>5.1261630555013333</v>
       </c>
       <c r="E263" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F263" t="s">
         <v>19</v>
@@ -14247,7 +14226,7 @@
         <v>5.7035591124991862</v>
       </c>
       <c r="E264" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F264" t="s">
         <v>19</v>
@@ -14272,7 +14251,7 @@
         <v>5.6222265599583574</v>
       </c>
       <c r="E265" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F265" t="s">
         <v>19</v>
@@ -14297,7 +14276,7 @@
         <v>6.1446418114386088</v>
       </c>
       <c r="E266" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F266" t="s">
         <v>19</v>
@@ -14322,7 +14301,7 @@
         <v>4.5001626651050808</v>
       </c>
       <c r="E267" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F267" t="s">
         <v>19</v>
@@ -14347,7 +14326,7 @@
         <v>1.6877480642852491</v>
       </c>
       <c r="E268" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F268" t="s">
         <v>19</v>
@@ -14372,7 +14351,7 @@
         <v>2.1458780662372305</v>
       </c>
       <c r="E269" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F269" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
first draft of dark vs light CL zone figures
Calculations done, will make nicer plots
- removed duplicate row from J100 "light" data
</commit_message>
<xml_diff>
--- a/CL Brightness DUvsDTh mol%.xlsx
+++ b/CL Brightness DUvsDTh mol%.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/DUDThZircon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CF48B0-5A3D-5F44-A61E-CF31F7D830DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39561364-1AD6-4845-97C1-2ED5B6C27B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="1300" windowWidth="28180" windowHeight="27500" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
+    <workbookView xWindow="4880" yWindow="1300" windowWidth="28180" windowHeight="27500" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="275">
   <si>
     <t>DARK</t>
   </si>
@@ -8042,14 +8042,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F37500E-3173-B64C-94B9-2EBED4B5FAA5}">
-  <dimension ref="A1:H272"/>
+  <dimension ref="A1:H271"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178:XFD178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11404,11 +11405,11 @@
         <v>100</v>
       </c>
       <c r="G145">
-        <f t="shared" ref="G145:G208" si="6">B145</f>
+        <f t="shared" ref="G145:G207" si="6">B145</f>
         <v>3.9347088812056485</v>
       </c>
       <c r="H145">
-        <f t="shared" ref="H145:H208" si="7">C145</f>
+        <f t="shared" ref="H145:H207" si="7">C145</f>
         <v>2.0046639674564561</v>
       </c>
     </row>
@@ -12180,13 +12181,13 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B178">
-        <v>1.7075596613468929</v>
+        <v>1.348999479027132</v>
       </c>
       <c r="C178">
-        <v>0.95630689055293971</v>
+        <v>0.6837605941472884</v>
       </c>
       <c r="E178" t="s">
         <v>272</v>
@@ -12196,22 +12197,22 @@
       </c>
       <c r="G178">
         <f t="shared" si="6"/>
-        <v>1.7075596613468929</v>
+        <v>1.348999479027132</v>
       </c>
       <c r="H178">
         <f t="shared" si="7"/>
-        <v>0.95630689055293971</v>
+        <v>0.6837605941472884</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B179">
-        <v>1.348999479027132</v>
+        <v>1.0893919139694852</v>
       </c>
       <c r="C179">
-        <v>0.6837605941472884</v>
+        <v>0.53012048252772936</v>
       </c>
       <c r="E179" t="s">
         <v>272</v>
@@ -12221,22 +12222,22 @@
       </c>
       <c r="G179">
         <f t="shared" si="6"/>
-        <v>1.348999479027132</v>
+        <v>1.0893919139694852</v>
       </c>
       <c r="H179">
         <f t="shared" si="7"/>
-        <v>0.6837605941472884</v>
+        <v>0.53012048252772936</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B180">
-        <v>1.0893919139694852</v>
+        <v>1.2221558863068664</v>
       </c>
       <c r="C180">
-        <v>0.53012048252772936</v>
+        <v>0.59310499880298861</v>
       </c>
       <c r="E180" t="s">
         <v>272</v>
@@ -12246,22 +12247,22 @@
       </c>
       <c r="G180">
         <f t="shared" si="6"/>
-        <v>1.0893919139694852</v>
+        <v>1.2221558863068664</v>
       </c>
       <c r="H180">
         <f t="shared" si="7"/>
-        <v>0.53012048252772936</v>
+        <v>0.59310499880298861</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B181">
-        <v>1.2221558863068664</v>
+        <v>1.0405609528208777</v>
       </c>
       <c r="C181">
-        <v>0.59310499880298861</v>
+        <v>0.48240967740857427</v>
       </c>
       <c r="E181" t="s">
         <v>272</v>
@@ -12271,22 +12272,22 @@
       </c>
       <c r="G181">
         <f t="shared" si="6"/>
-        <v>1.2221558863068664</v>
+        <v>1.0405609528208777</v>
       </c>
       <c r="H181">
         <f t="shared" si="7"/>
-        <v>0.59310499880298861</v>
+        <v>0.48240967740857427</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
-        <v>175</v>
+      <c r="A182" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B182">
-        <v>1.0405609528208777</v>
+        <v>1.0840149762716718</v>
       </c>
       <c r="C182">
-        <v>0.48240967740857427</v>
+        <v>0.45824666440791362</v>
       </c>
       <c r="E182" t="s">
         <v>272</v>
@@ -12296,22 +12297,22 @@
       </c>
       <c r="G182">
         <f t="shared" si="6"/>
-        <v>1.0405609528208777</v>
+        <v>1.0840149762716718</v>
       </c>
       <c r="H182">
         <f t="shared" si="7"/>
-        <v>0.48240967740857427</v>
+        <v>0.45824666440791362</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B183">
-        <v>1.0840149762716718</v>
+        <v>0.91784513390408529</v>
       </c>
       <c r="C183">
-        <v>0.45824666440791362</v>
+        <v>0.42640682429331767</v>
       </c>
       <c r="E183" t="s">
         <v>272</v>
@@ -12321,52 +12322,52 @@
       </c>
       <c r="G183">
         <f t="shared" si="6"/>
-        <v>1.0840149762716718</v>
+        <v>0.91784513390408529</v>
       </c>
       <c r="H183">
         <f t="shared" si="7"/>
-        <v>0.45824666440791362</v>
+        <v>0.42640682429331767</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A184" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B184">
-        <v>0.91784513390408529</v>
-      </c>
-      <c r="C184">
-        <v>0.42640682429331767</v>
-      </c>
-      <c r="E184" t="s">
-        <v>272</v>
-      </c>
-      <c r="F184" t="s">
-        <v>19</v>
-      </c>
-      <c r="G184">
-        <f t="shared" si="6"/>
-        <v>0.91784513390408529</v>
-      </c>
-      <c r="H184">
-        <f t="shared" si="7"/>
-        <v>0.42640682429331767</v>
+      <c r="A184" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>0</v>
+        <v>178</v>
+      </c>
+      <c r="B185">
+        <v>1.7004257104810614</v>
+      </c>
+      <c r="C185">
+        <v>1.3920827437358692</v>
+      </c>
+      <c r="E185" t="s">
+        <v>272</v>
+      </c>
+      <c r="F185" t="s">
+        <v>100</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="6"/>
+        <v>1.7004257104810614</v>
+      </c>
+      <c r="H185">
+        <f t="shared" si="7"/>
+        <v>1.3920827437358692</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B186">
-        <v>1.7004257104810614</v>
+        <v>2.6154508168395196</v>
       </c>
       <c r="C186">
-        <v>1.3920827437358692</v>
+        <v>2.6344470538032265</v>
       </c>
       <c r="E186" t="s">
         <v>272</v>
@@ -12376,22 +12377,22 @@
       </c>
       <c r="G186">
         <f t="shared" si="6"/>
-        <v>1.7004257104810614</v>
+        <v>2.6154508168395196</v>
       </c>
       <c r="H186">
         <f t="shared" si="7"/>
-        <v>1.3920827437358692</v>
+        <v>2.6344470538032265</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B187">
-        <v>2.6154508168395196</v>
+        <v>1.6044020703158963</v>
       </c>
       <c r="C187">
-        <v>2.6344470538032265</v>
+        <v>1.2876573659521637</v>
       </c>
       <c r="E187" t="s">
         <v>272</v>
@@ -12401,22 +12402,22 @@
       </c>
       <c r="G187">
         <f t="shared" si="6"/>
-        <v>2.6154508168395196</v>
+        <v>1.6044020703158963</v>
       </c>
       <c r="H187">
         <f t="shared" si="7"/>
-        <v>2.6344470538032265</v>
+        <v>1.2876573659521637</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B188">
-        <v>1.6044020703158963</v>
+        <v>2.5691431985732214</v>
       </c>
       <c r="C188">
-        <v>1.2876573659521637</v>
+        <v>2.9463274148742036</v>
       </c>
       <c r="E188" t="s">
         <v>272</v>
@@ -12426,22 +12427,22 @@
       </c>
       <c r="G188">
         <f t="shared" si="6"/>
-        <v>1.6044020703158963</v>
+        <v>2.5691431985732214</v>
       </c>
       <c r="H188">
         <f t="shared" si="7"/>
-        <v>1.2876573659521637</v>
+        <v>2.9463274148742036</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B189">
-        <v>2.5691431985732214</v>
+        <v>1.9876922124160095</v>
       </c>
       <c r="C189">
-        <v>2.9463274148742036</v>
+        <v>1.9018095272570115</v>
       </c>
       <c r="E189" t="s">
         <v>272</v>
@@ -12451,22 +12452,22 @@
       </c>
       <c r="G189">
         <f t="shared" si="6"/>
-        <v>2.5691431985732214</v>
+        <v>1.9876922124160095</v>
       </c>
       <c r="H189">
         <f t="shared" si="7"/>
-        <v>2.9463274148742036</v>
+        <v>1.9018095272570115</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B190">
-        <v>1.9876922124160095</v>
+        <v>3.2549248957857198</v>
       </c>
       <c r="C190">
-        <v>1.9018095272570115</v>
+        <v>4.0094681904869027</v>
       </c>
       <c r="E190" t="s">
         <v>272</v>
@@ -12476,22 +12477,22 @@
       </c>
       <c r="G190">
         <f t="shared" si="6"/>
-        <v>1.9876922124160095</v>
+        <v>3.2549248957857198</v>
       </c>
       <c r="H190">
         <f t="shared" si="7"/>
-        <v>1.9018095272570115</v>
+        <v>4.0094681904869027</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B191">
-        <v>3.2549248957857198</v>
+        <v>1.9269010932845385</v>
       </c>
       <c r="C191">
-        <v>4.0094681904869027</v>
+        <v>1.9458432739560734</v>
       </c>
       <c r="E191" t="s">
         <v>272</v>
@@ -12501,22 +12502,22 @@
       </c>
       <c r="G191">
         <f t="shared" si="6"/>
-        <v>3.2549248957857198</v>
+        <v>1.9269010932845385</v>
       </c>
       <c r="H191">
         <f t="shared" si="7"/>
-        <v>4.0094681904869027</v>
+        <v>1.9458432739560734</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B192">
-        <v>1.9269010932845385</v>
+        <v>2.0116608838422843</v>
       </c>
       <c r="C192">
-        <v>1.9458432739560734</v>
+        <v>1.6992265822360058</v>
       </c>
       <c r="E192" t="s">
         <v>272</v>
@@ -12526,22 +12527,22 @@
       </c>
       <c r="G192">
         <f t="shared" si="6"/>
-        <v>1.9269010932845385</v>
+        <v>2.0116608838422843</v>
       </c>
       <c r="H192">
         <f t="shared" si="7"/>
-        <v>1.9458432739560734</v>
+        <v>1.6992265822360058</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B193">
-        <v>2.0116608838422843</v>
+        <v>4.0025347299912308</v>
       </c>
       <c r="C193">
-        <v>1.6992265822360058</v>
+        <v>4.9781564054012133</v>
       </c>
       <c r="E193" t="s">
         <v>272</v>
@@ -12551,22 +12552,22 @@
       </c>
       <c r="G193">
         <f t="shared" si="6"/>
-        <v>2.0116608838422843</v>
+        <v>4.0025347299912308</v>
       </c>
       <c r="H193">
         <f t="shared" si="7"/>
-        <v>1.6992265822360058</v>
+        <v>4.9781564054012133</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B194">
-        <v>4.0025347299912308</v>
+        <v>1.9876922366812912</v>
       </c>
       <c r="C194">
-        <v>4.9781564054012133</v>
+        <v>2.0363160049914404</v>
       </c>
       <c r="E194" t="s">
         <v>272</v>
@@ -12576,22 +12577,22 @@
       </c>
       <c r="G194">
         <f t="shared" si="6"/>
-        <v>4.0025347299912308</v>
+        <v>1.9876922366812912</v>
       </c>
       <c r="H194">
         <f t="shared" si="7"/>
-        <v>4.9781564054012133</v>
+        <v>2.0363160049914404</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B195">
-        <v>1.9876922366812912</v>
+        <v>1.7274889096805242</v>
       </c>
       <c r="C195">
-        <v>2.0363160049914404</v>
+        <v>1.5311194345723143</v>
       </c>
       <c r="E195" t="s">
         <v>272</v>
@@ -12601,22 +12602,22 @@
       </c>
       <c r="G195">
         <f t="shared" si="6"/>
-        <v>1.9876922366812912</v>
+        <v>1.7274889096805242</v>
       </c>
       <c r="H195">
         <f t="shared" si="7"/>
-        <v>2.0363160049914404</v>
+        <v>1.5311194345723143</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B196">
-        <v>1.7274889096805242</v>
+        <v>3.7979159736016461</v>
       </c>
       <c r="C196">
-        <v>1.5311194345723143</v>
+        <v>4.4436379592518627</v>
       </c>
       <c r="E196" t="s">
         <v>272</v>
@@ -12626,22 +12627,22 @@
       </c>
       <c r="G196">
         <f t="shared" si="6"/>
-        <v>1.7274889096805242</v>
+        <v>3.7979159736016461</v>
       </c>
       <c r="H196">
         <f t="shared" si="7"/>
-        <v>1.5311194345723143</v>
+        <v>4.4436379592518627</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B197">
-        <v>3.7979159736016461</v>
+        <v>5.181949413581072</v>
       </c>
       <c r="C197">
-        <v>4.4436379592518627</v>
+        <v>6.5106315940233568</v>
       </c>
       <c r="E197" t="s">
         <v>272</v>
@@ -12651,22 +12652,22 @@
       </c>
       <c r="G197">
         <f t="shared" si="6"/>
-        <v>3.7979159736016461</v>
+        <v>5.181949413581072</v>
       </c>
       <c r="H197">
         <f t="shared" si="7"/>
-        <v>4.4436379592518627</v>
+        <v>6.5106315940233568</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B198">
-        <v>5.181949413581072</v>
+        <v>2.6577489935495389</v>
       </c>
       <c r="C198">
-        <v>6.5106315940233568</v>
+        <v>2.1054257091840332</v>
       </c>
       <c r="E198" t="s">
         <v>272</v>
@@ -12676,22 +12677,22 @@
       </c>
       <c r="G198">
         <f t="shared" si="6"/>
-        <v>5.181949413581072</v>
+        <v>2.6577489935495389</v>
       </c>
       <c r="H198">
         <f t="shared" si="7"/>
-        <v>6.5106315940233568</v>
+        <v>2.1054257091840332</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B199">
-        <v>2.6577489935495389</v>
+        <v>3.4950741419299312</v>
       </c>
       <c r="C199">
-        <v>2.1054257091840332</v>
+        <v>2.89553894691355</v>
       </c>
       <c r="E199" t="s">
         <v>272</v>
@@ -12701,22 +12702,22 @@
       </c>
       <c r="G199">
         <f t="shared" si="6"/>
-        <v>2.6577489935495389</v>
+        <v>3.4950741419299312</v>
       </c>
       <c r="H199">
         <f t="shared" si="7"/>
-        <v>2.1054257091840332</v>
+        <v>2.89553894691355</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B200">
-        <v>3.4950741419299312</v>
+        <v>2.5664662237718172</v>
       </c>
       <c r="C200">
-        <v>2.89553894691355</v>
+        <v>2.4069171308235857</v>
       </c>
       <c r="E200" t="s">
         <v>272</v>
@@ -12726,22 +12727,22 @@
       </c>
       <c r="G200">
         <f t="shared" si="6"/>
-        <v>3.4950741419299312</v>
+        <v>2.5664662237718172</v>
       </c>
       <c r="H200">
         <f t="shared" si="7"/>
-        <v>2.89553894691355</v>
+        <v>2.4069171308235857</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B201">
-        <v>2.5664662237718172</v>
+        <v>2.3724401682649909</v>
       </c>
       <c r="C201">
-        <v>2.4069171308235857</v>
+        <v>1.7553715061227722</v>
       </c>
       <c r="E201" t="s">
         <v>272</v>
@@ -12751,22 +12752,22 @@
       </c>
       <c r="G201">
         <f t="shared" si="6"/>
-        <v>2.5664662237718172</v>
+        <v>2.3724401682649909</v>
       </c>
       <c r="H201">
         <f t="shared" si="7"/>
-        <v>2.4069171308235857</v>
+        <v>1.7553715061227722</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B202">
-        <v>2.3724401682649909</v>
+        <v>2.6036892462315508</v>
       </c>
       <c r="C202">
-        <v>1.7553715061227722</v>
+        <v>2.3839342911860308</v>
       </c>
       <c r="E202" t="s">
         <v>272</v>
@@ -12776,22 +12777,22 @@
       </c>
       <c r="G202">
         <f t="shared" si="6"/>
-        <v>2.3724401682649909</v>
+        <v>2.6036892462315508</v>
       </c>
       <c r="H202">
         <f t="shared" si="7"/>
-        <v>1.7553715061227722</v>
+        <v>2.3839342911860308</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B203">
-        <v>2.6036892462315508</v>
+        <v>2.2767402197653959</v>
       </c>
       <c r="C203">
-        <v>2.3839342911860308</v>
+        <v>1.7945396109667138</v>
       </c>
       <c r="E203" t="s">
         <v>272</v>
@@ -12801,22 +12802,22 @@
       </c>
       <c r="G203">
         <f t="shared" si="6"/>
-        <v>2.6036892462315508</v>
+        <v>2.2767402197653959</v>
       </c>
       <c r="H203">
         <f t="shared" si="7"/>
-        <v>2.3839342911860308</v>
+        <v>1.7945396109667138</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B204">
-        <v>2.2767402197653959</v>
+        <v>2.1477782480022607</v>
       </c>
       <c r="C204">
-        <v>1.7945396109667138</v>
+        <v>1.6212395523817154</v>
       </c>
       <c r="E204" t="s">
         <v>272</v>
@@ -12826,22 +12827,22 @@
       </c>
       <c r="G204">
         <f t="shared" si="6"/>
-        <v>2.2767402197653959</v>
+        <v>2.1477782480022607</v>
       </c>
       <c r="H204">
         <f t="shared" si="7"/>
-        <v>1.7945396109667138</v>
+        <v>1.6212395523817154</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B205">
-        <v>2.1477782480022607</v>
+        <v>3.6668725630311956</v>
       </c>
       <c r="C205">
-        <v>1.6212395523817154</v>
+        <v>3.2259945716254927</v>
       </c>
       <c r="E205" t="s">
         <v>272</v>
@@ -12851,22 +12852,22 @@
       </c>
       <c r="G205">
         <f t="shared" si="6"/>
-        <v>2.1477782480022607</v>
+        <v>3.6668725630311956</v>
       </c>
       <c r="H205">
         <f t="shared" si="7"/>
-        <v>1.6212395523817154</v>
+        <v>3.2259945716254927</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B206">
-        <v>3.6668725630311956</v>
+        <v>2.2608237150272918</v>
       </c>
       <c r="C206">
-        <v>3.2259945716254927</v>
+        <v>2.0069326735774244</v>
       </c>
       <c r="E206" t="s">
         <v>272</v>
@@ -12876,22 +12877,22 @@
       </c>
       <c r="G206">
         <f t="shared" si="6"/>
-        <v>3.6668725630311956</v>
+        <v>2.2608237150272918</v>
       </c>
       <c r="H206">
         <f t="shared" si="7"/>
-        <v>3.2259945716254927</v>
+        <v>2.0069326735774244</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A207" s="1" t="s">
-        <v>199</v>
+      <c r="A207" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="B207">
-        <v>2.2608237150272918</v>
+        <v>2.7016430973219192</v>
       </c>
       <c r="C207">
-        <v>2.0069326735774244</v>
+        <v>2.143013376678518</v>
       </c>
       <c r="E207" t="s">
         <v>272</v>
@@ -12901,22 +12902,22 @@
       </c>
       <c r="G207">
         <f t="shared" si="6"/>
-        <v>2.2608237150272918</v>
+        <v>2.7016430973219192</v>
       </c>
       <c r="H207">
         <f t="shared" si="7"/>
-        <v>2.0069326735774244</v>
+        <v>2.143013376678518</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B208">
-        <v>2.7016430973219192</v>
+        <v>1.0897383921970765</v>
       </c>
       <c r="C208">
-        <v>2.143013376678518</v>
+        <v>0.62554306569969165</v>
       </c>
       <c r="E208" t="s">
         <v>272</v>
@@ -12925,59 +12926,59 @@
         <v>100</v>
       </c>
       <c r="G208">
-        <f t="shared" si="6"/>
-        <v>2.7016430973219192</v>
+        <f t="shared" ref="G208:G268" si="8">B208</f>
+        <v>1.0897383921970765</v>
       </c>
       <c r="H208">
-        <f t="shared" si="7"/>
-        <v>2.143013376678518</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B209">
-        <v>1.0897383921970765</v>
-      </c>
-      <c r="C209">
+        <f t="shared" ref="H208:H268" si="9">C208</f>
         <v>0.62554306569969165</v>
       </c>
-      <c r="E209" t="s">
-        <v>272</v>
-      </c>
-      <c r="F209" t="s">
-        <v>100</v>
-      </c>
-      <c r="G209">
-        <f t="shared" ref="G209:G269" si="8">B209</f>
-        <v>1.0897383921970765</v>
-      </c>
-      <c r="H209">
-        <f t="shared" ref="H209:H269" si="9">C209</f>
-        <v>0.62554306569969165</v>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B210" t="s">
+        <v>17</v>
+      </c>
+      <c r="C210" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B211" t="s">
-        <v>17</v>
-      </c>
-      <c r="C211" t="s">
-        <v>18</v>
+      <c r="A211" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B211">
+        <v>2.0308980268430012</v>
+      </c>
+      <c r="C211">
+        <v>1.0857185123673931</v>
+      </c>
+      <c r="E211" t="s">
+        <v>273</v>
+      </c>
+      <c r="F211" t="s">
+        <v>19</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="8"/>
+        <v>2.0308980268430012</v>
+      </c>
+      <c r="H211">
+        <f t="shared" si="9"/>
+        <v>1.0857185123673931</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B212">
-        <v>2.0308980268430012</v>
+        <v>1.1876426852989261</v>
       </c>
       <c r="C212">
-        <v>1.0857185123673931</v>
+        <v>0.65377352480922901</v>
       </c>
       <c r="E212" t="s">
         <v>273</v>
@@ -12987,22 +12988,22 @@
       </c>
       <c r="G212">
         <f t="shared" si="8"/>
-        <v>2.0308980268430012</v>
+        <v>1.1876426852989261</v>
       </c>
       <c r="H212">
         <f t="shared" si="9"/>
-        <v>1.0857185123673931</v>
+        <v>0.65377352480922901</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B213">
-        <v>1.1876426852989261</v>
+        <v>1.1084384648078294</v>
       </c>
       <c r="C213">
-        <v>0.65377352480922901</v>
+        <v>0.70066379308607007</v>
       </c>
       <c r="E213" t="s">
         <v>273</v>
@@ -13012,22 +13013,22 @@
       </c>
       <c r="G213">
         <f t="shared" si="8"/>
-        <v>1.1876426852989261</v>
+        <v>1.1084384648078294</v>
       </c>
       <c r="H213">
         <f t="shared" si="9"/>
-        <v>0.65377352480922901</v>
+        <v>0.70066379308607007</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B214">
-        <v>1.1084384648078294</v>
+        <v>2.1161375273272336</v>
       </c>
       <c r="C214">
-        <v>0.70066379308607007</v>
+        <v>1.3533683779214274</v>
       </c>
       <c r="E214" t="s">
         <v>273</v>
@@ -13037,22 +13038,22 @@
       </c>
       <c r="G214">
         <f t="shared" si="8"/>
-        <v>1.1084384648078294</v>
+        <v>2.1161375273272336</v>
       </c>
       <c r="H214">
         <f t="shared" si="9"/>
-        <v>0.70066379308607007</v>
+        <v>1.3533683779214274</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B215">
-        <v>2.1161375273272336</v>
+        <v>1.6177205257247642</v>
       </c>
       <c r="C215">
-        <v>1.3533683779214274</v>
+        <v>0.80089753392428087</v>
       </c>
       <c r="E215" t="s">
         <v>273</v>
@@ -13062,22 +13063,22 @@
       </c>
       <c r="G215">
         <f t="shared" si="8"/>
-        <v>2.1161375273272336</v>
+        <v>1.6177205257247642</v>
       </c>
       <c r="H215">
         <f t="shared" si="9"/>
-        <v>1.3533683779214274</v>
+        <v>0.80089753392428087</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B216">
-        <v>1.6177205257247642</v>
+        <v>1.0430286293256796</v>
       </c>
       <c r="C216">
-        <v>0.80089753392428087</v>
+        <v>0.57134640411045745</v>
       </c>
       <c r="E216" t="s">
         <v>273</v>
@@ -13087,22 +13088,22 @@
       </c>
       <c r="G216">
         <f t="shared" si="8"/>
-        <v>1.6177205257247642</v>
+        <v>1.0430286293256796</v>
       </c>
       <c r="H216">
         <f t="shared" si="9"/>
-        <v>0.80089753392428087</v>
+        <v>0.57134640411045745</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B217">
-        <v>1.0430286293256796</v>
+        <v>2.2385808162301037</v>
       </c>
       <c r="C217">
-        <v>0.57134640411045745</v>
+        <v>1.3055403788057476</v>
       </c>
       <c r="E217" t="s">
         <v>273</v>
@@ -13112,22 +13113,22 @@
       </c>
       <c r="G217">
         <f t="shared" si="8"/>
-        <v>1.0430286293256796</v>
+        <v>2.2385808162301037</v>
       </c>
       <c r="H217">
         <f t="shared" si="9"/>
-        <v>0.57134640411045745</v>
+        <v>1.3055403788057476</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B218">
-        <v>2.2385808162301037</v>
+        <v>1.6635811464226784</v>
       </c>
       <c r="C218">
-        <v>1.3055403788057476</v>
+        <v>1.0028688214512544</v>
       </c>
       <c r="E218" t="s">
         <v>273</v>
@@ -13137,22 +13138,22 @@
       </c>
       <c r="G218">
         <f t="shared" si="8"/>
-        <v>2.2385808162301037</v>
+        <v>1.6635811464226784</v>
       </c>
       <c r="H218">
         <f t="shared" si="9"/>
-        <v>1.3055403788057476</v>
+        <v>1.0028688214512544</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A219" s="1" t="s">
-        <v>209</v>
+      <c r="A219" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="B219">
-        <v>1.6635811464226784</v>
+        <v>1.755799002211593</v>
       </c>
       <c r="C219">
-        <v>1.0028688214512544</v>
+        <v>1.231979445145589</v>
       </c>
       <c r="E219" t="s">
         <v>273</v>
@@ -13162,22 +13163,22 @@
       </c>
       <c r="G219">
         <f t="shared" si="8"/>
-        <v>1.6635811464226784</v>
+        <v>1.755799002211593</v>
       </c>
       <c r="H219">
         <f t="shared" si="9"/>
-        <v>1.0028688214512544</v>
+        <v>1.231979445145589</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B220">
-        <v>1.755799002211593</v>
+        <v>2.0352826209947024</v>
       </c>
       <c r="C220">
-        <v>1.231979445145589</v>
+        <v>1.8126857468550253</v>
       </c>
       <c r="E220" t="s">
         <v>273</v>
@@ -13187,22 +13188,22 @@
       </c>
       <c r="G220">
         <f t="shared" si="8"/>
-        <v>1.755799002211593</v>
+        <v>2.0352826209947024</v>
       </c>
       <c r="H220">
         <f t="shared" si="9"/>
-        <v>1.231979445145589</v>
+        <v>1.8126857468550253</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B221">
-        <v>2.0352826209947024</v>
+        <v>1.0457233965951758</v>
       </c>
       <c r="C221">
-        <v>1.8126857468550253</v>
+        <v>1.0689700407568743</v>
       </c>
       <c r="E221" t="s">
         <v>273</v>
@@ -13212,52 +13213,52 @@
       </c>
       <c r="G221">
         <f t="shared" si="8"/>
-        <v>2.0352826209947024</v>
+        <v>1.0457233965951758</v>
       </c>
       <c r="H221">
         <f t="shared" si="9"/>
-        <v>1.8126857468550253</v>
+        <v>1.0689700407568743</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B222">
-        <v>1.0457233965951758</v>
-      </c>
-      <c r="C222">
-        <v>1.0689700407568743</v>
-      </c>
-      <c r="E222" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B223">
+        <v>1.4097318655816309</v>
+      </c>
+      <c r="C223">
+        <v>1.1753100485560408</v>
+      </c>
+      <c r="E223" t="s">
         <v>273</v>
       </c>
-      <c r="F222" t="s">
-        <v>19</v>
-      </c>
-      <c r="G222">
+      <c r="F223" t="s">
+        <v>100</v>
+      </c>
+      <c r="G223">
         <f t="shared" si="8"/>
-        <v>1.0457233965951758</v>
-      </c>
-      <c r="H222">
+        <v>1.4097318655816309</v>
+      </c>
+      <c r="H223">
         <f t="shared" si="9"/>
-        <v>1.0689700407568743</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A223" s="2" t="s">
-        <v>100</v>
+        <v>1.1753100485560408</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B224">
-        <v>1.4097318655816309</v>
+        <v>2.2697724844757681</v>
       </c>
       <c r="C224">
-        <v>1.1753100485560408</v>
+        <v>1.8628343431388317</v>
       </c>
       <c r="E224" t="s">
         <v>273</v>
@@ -13267,22 +13268,22 @@
       </c>
       <c r="G224">
         <f t="shared" si="8"/>
-        <v>1.4097318655816309</v>
+        <v>2.2697724844757681</v>
       </c>
       <c r="H224">
         <f t="shared" si="9"/>
-        <v>1.1753100485560408</v>
+        <v>1.8628343431388317</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B225">
-        <v>2.2697724844757681</v>
+        <v>1.1692489809574942</v>
       </c>
       <c r="C225">
-        <v>1.8628343431388317</v>
+        <v>1.2045903552921469</v>
       </c>
       <c r="E225" t="s">
         <v>273</v>
@@ -13292,22 +13293,22 @@
       </c>
       <c r="G225">
         <f t="shared" si="8"/>
-        <v>2.2697724844757681</v>
+        <v>1.1692489809574942</v>
       </c>
       <c r="H225">
         <f t="shared" si="9"/>
-        <v>1.8628343431388317</v>
+        <v>1.2045903552921469</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B226">
-        <v>1.1692489809574942</v>
+        <v>1.3229137147687682</v>
       </c>
       <c r="C226">
-        <v>1.2045903552921469</v>
+        <v>1.319218266035356</v>
       </c>
       <c r="E226" t="s">
         <v>273</v>
@@ -13317,22 +13318,22 @@
       </c>
       <c r="G226">
         <f t="shared" si="8"/>
-        <v>1.1692489809574942</v>
+        <v>1.3229137147687682</v>
       </c>
       <c r="H226">
         <f t="shared" si="9"/>
-        <v>1.2045903552921469</v>
+        <v>1.319218266035356</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B227">
-        <v>1.3229137147687682</v>
+        <v>3.2432788396215382</v>
       </c>
       <c r="C227">
-        <v>1.319218266035356</v>
+        <v>2.6970677264530059</v>
       </c>
       <c r="E227" t="s">
         <v>273</v>
@@ -13342,22 +13343,22 @@
       </c>
       <c r="G227">
         <f t="shared" si="8"/>
-        <v>1.3229137147687682</v>
+        <v>3.2432788396215382</v>
       </c>
       <c r="H227">
         <f t="shared" si="9"/>
-        <v>1.319218266035356</v>
+        <v>2.6970677264530059</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B228">
-        <v>3.2432788396215382</v>
+        <v>1.0643732593227335</v>
       </c>
       <c r="C228">
-        <v>2.6970677264530059</v>
+        <v>0.78992000766093473</v>
       </c>
       <c r="E228" t="s">
         <v>273</v>
@@ -13367,22 +13368,22 @@
       </c>
       <c r="G228">
         <f t="shared" si="8"/>
-        <v>3.2432788396215382</v>
+        <v>1.0643732593227335</v>
       </c>
       <c r="H228">
         <f t="shared" si="9"/>
-        <v>2.6970677264530059</v>
+        <v>0.78992000766093473</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B229">
-        <v>1.0643732593227335</v>
+        <v>1.6323012951203184</v>
       </c>
       <c r="C229">
-        <v>0.78992000766093473</v>
+        <v>1.3883916626658384</v>
       </c>
       <c r="E229" t="s">
         <v>273</v>
@@ -13392,22 +13393,22 @@
       </c>
       <c r="G229">
         <f t="shared" si="8"/>
-        <v>1.0643732593227335</v>
+        <v>1.6323012951203184</v>
       </c>
       <c r="H229">
         <f t="shared" si="9"/>
-        <v>0.78992000766093473</v>
+        <v>1.3883916626658384</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B230">
-        <v>1.6323012951203184</v>
+        <v>1.7849397066215145</v>
       </c>
       <c r="C230">
-        <v>1.3883916626658384</v>
+        <v>1.4373497113544722</v>
       </c>
       <c r="E230" t="s">
         <v>273</v>
@@ -13417,22 +13418,22 @@
       </c>
       <c r="G230">
         <f t="shared" si="8"/>
-        <v>1.6323012951203184</v>
+        <v>1.7849397066215145</v>
       </c>
       <c r="H230">
         <f t="shared" si="9"/>
-        <v>1.3883916626658384</v>
+        <v>1.4373497113544722</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B231">
-        <v>1.7849397066215145</v>
+        <v>1.6131256987016713</v>
       </c>
       <c r="C231">
-        <v>1.4373497113544722</v>
+        <v>1.1543557351309801</v>
       </c>
       <c r="E231" t="s">
         <v>273</v>
@@ -13442,22 +13443,22 @@
       </c>
       <c r="G231">
         <f t="shared" si="8"/>
-        <v>1.7849397066215145</v>
+        <v>1.6131256987016713</v>
       </c>
       <c r="H231">
         <f t="shared" si="9"/>
-        <v>1.4373497113544722</v>
+        <v>1.1543557351309801</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B232">
-        <v>1.6131256987016713</v>
+        <v>1.9482182782134649</v>
       </c>
       <c r="C232">
-        <v>1.1543557351309801</v>
+        <v>1.6285222852443999</v>
       </c>
       <c r="E232" t="s">
         <v>273</v>
@@ -13467,22 +13468,22 @@
       </c>
       <c r="G232">
         <f t="shared" si="8"/>
-        <v>1.6131256987016713</v>
+        <v>1.9482182782134649</v>
       </c>
       <c r="H232">
         <f t="shared" si="9"/>
-        <v>1.1543557351309801</v>
+        <v>1.6285222852443999</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B233">
-        <v>1.9482182782134649</v>
+        <v>3.0136807982095024</v>
       </c>
       <c r="C233">
-        <v>1.6285222852443999</v>
+        <v>2.3901841722256312</v>
       </c>
       <c r="E233" t="s">
         <v>273</v>
@@ -13492,22 +13493,22 @@
       </c>
       <c r="G233">
         <f t="shared" si="8"/>
-        <v>1.9482182782134649</v>
+        <v>3.0136807982095024</v>
       </c>
       <c r="H233">
         <f t="shared" si="9"/>
-        <v>1.6285222852443999</v>
+        <v>2.3901841722256312</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B234">
-        <v>3.0136807982095024</v>
+        <v>1.9658087308233883</v>
       </c>
       <c r="C234">
-        <v>2.3901841722256312</v>
+        <v>1.6099626707873229</v>
       </c>
       <c r="E234" t="s">
         <v>273</v>
@@ -13517,22 +13518,22 @@
       </c>
       <c r="G234">
         <f t="shared" si="8"/>
-        <v>3.0136807982095024</v>
+        <v>1.9658087308233883</v>
       </c>
       <c r="H234">
         <f t="shared" si="9"/>
-        <v>2.3901841722256312</v>
+        <v>1.6099626707873229</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A235" s="1" t="s">
-        <v>224</v>
+      <c r="A235" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="B235">
-        <v>1.9658087308233883</v>
+        <v>2.4632001234377414</v>
       </c>
       <c r="C235">
-        <v>1.6099626707873229</v>
+        <v>2.3303523366219281</v>
       </c>
       <c r="E235" t="s">
         <v>273</v>
@@ -13542,22 +13543,22 @@
       </c>
       <c r="G235">
         <f t="shared" si="8"/>
-        <v>1.9658087308233883</v>
+        <v>2.4632001234377414</v>
       </c>
       <c r="H235">
         <f t="shared" si="9"/>
-        <v>1.6099626707873229</v>
+        <v>2.3303523366219281</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B236">
-        <v>2.4632001234377414</v>
+        <v>1.731060021601605</v>
       </c>
       <c r="C236">
-        <v>2.3303523366219281</v>
+        <v>1.7068942899663897</v>
       </c>
       <c r="E236" t="s">
         <v>273</v>
@@ -13567,22 +13568,22 @@
       </c>
       <c r="G236">
         <f t="shared" si="8"/>
-        <v>2.4632001234377414</v>
+        <v>1.731060021601605</v>
       </c>
       <c r="H236">
         <f t="shared" si="9"/>
-        <v>2.3303523366219281</v>
+        <v>1.7068942899663897</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B237">
-        <v>1.731060021601605</v>
+        <v>0.81036877025150444</v>
       </c>
       <c r="C237">
-        <v>1.7068942899663897</v>
+        <v>0.53301487784246382</v>
       </c>
       <c r="E237" t="s">
         <v>273</v>
@@ -13592,58 +13593,58 @@
       </c>
       <c r="G237">
         <f t="shared" si="8"/>
-        <v>1.731060021601605</v>
+        <v>0.81036877025150444</v>
       </c>
       <c r="H237">
         <f t="shared" si="9"/>
-        <v>1.7068942899663897</v>
+        <v>0.53301487784246382</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B238">
-        <v>0.81036877025150444</v>
-      </c>
-      <c r="C238">
-        <v>0.53301487784246382</v>
-      </c>
-      <c r="E238" t="s">
-        <v>273</v>
-      </c>
-      <c r="F238" t="s">
         <v>100</v>
       </c>
-      <c r="G238">
-        <f t="shared" si="8"/>
-        <v>0.81036877025150444</v>
-      </c>
-      <c r="H238">
-        <f t="shared" si="9"/>
-        <v>0.53301487784246382</v>
+      <c r="B238" t="s">
+        <v>257</v>
+      </c>
+      <c r="C238" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B239">
+        <v>3.3369963924036274</v>
+      </c>
+      <c r="C239">
+        <v>13.523716572320904</v>
+      </c>
+      <c r="E239" t="s">
+        <v>274</v>
+      </c>
+      <c r="F239" t="s">
         <v>100</v>
       </c>
-      <c r="B239" t="s">
-        <v>257</v>
-      </c>
-      <c r="C239" t="s">
-        <v>44</v>
+      <c r="G239">
+        <f t="shared" si="8"/>
+        <v>3.3369963924036274</v>
+      </c>
+      <c r="H239">
+        <f t="shared" si="9"/>
+        <v>13.523716572320904</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B240">
-        <v>3.3369963924036274</v>
+        <v>2.6677834837128742</v>
       </c>
       <c r="C240">
-        <v>13.523716572320904</v>
+        <v>7.4400416422669</v>
       </c>
       <c r="E240" t="s">
         <v>274</v>
@@ -13653,22 +13654,22 @@
       </c>
       <c r="G240">
         <f t="shared" si="8"/>
-        <v>3.3369963924036274</v>
+        <v>2.6677834837128742</v>
       </c>
       <c r="H240">
         <f t="shared" si="9"/>
-        <v>13.523716572320904</v>
+        <v>7.4400416422669</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B241">
-        <v>2.6677834837128742</v>
+        <v>2.2258567095998365</v>
       </c>
       <c r="C241">
-        <v>7.4400416422669</v>
+        <v>4.4377643307957566</v>
       </c>
       <c r="E241" t="s">
         <v>274</v>
@@ -13678,22 +13679,22 @@
       </c>
       <c r="G241">
         <f t="shared" si="8"/>
-        <v>2.6677834837128742</v>
+        <v>2.2258567095998365</v>
       </c>
       <c r="H241">
         <f t="shared" si="9"/>
-        <v>7.4400416422669</v>
+        <v>4.4377643307957566</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B242">
-        <v>2.2258567095998365</v>
+        <v>2.6787650978286353</v>
       </c>
       <c r="C242">
-        <v>4.4377643307957566</v>
+        <v>5.9510703363914361</v>
       </c>
       <c r="E242" t="s">
         <v>274</v>
@@ -13703,22 +13704,22 @@
       </c>
       <c r="G242">
         <f t="shared" si="8"/>
-        <v>2.2258567095998365</v>
+        <v>2.6787650978286353</v>
       </c>
       <c r="H242">
         <f t="shared" si="9"/>
-        <v>4.4377643307957566</v>
+        <v>5.9510703363914361</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B243">
-        <v>2.6787650978286353</v>
+        <v>4.0472239659358191</v>
       </c>
       <c r="C243">
-        <v>5.9510703363914361</v>
+        <v>10.973583186934738</v>
       </c>
       <c r="E243" t="s">
         <v>274</v>
@@ -13728,52 +13729,52 @@
       </c>
       <c r="G243">
         <f t="shared" si="8"/>
-        <v>2.6787650978286353</v>
+        <v>4.0472239659358191</v>
       </c>
       <c r="H243">
         <f t="shared" si="9"/>
-        <v>5.9510703363914361</v>
+        <v>10.973583186934738</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A244" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B244">
-        <v>4.0472239659358191</v>
-      </c>
-      <c r="C244">
-        <v>10.973583186934738</v>
-      </c>
-      <c r="E244" t="s">
+      <c r="A244" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B245">
+        <v>2.0895428260830022</v>
+      </c>
+      <c r="C245">
+        <v>6.0390396252195968</v>
+      </c>
+      <c r="E245" t="s">
         <v>274</v>
       </c>
-      <c r="F244" t="s">
-        <v>100</v>
-      </c>
-      <c r="G244">
+      <c r="F245" t="s">
+        <v>19</v>
+      </c>
+      <c r="G245">
         <f t="shared" si="8"/>
-        <v>4.0472239659358191</v>
-      </c>
-      <c r="H244">
+        <v>2.0895428260830022</v>
+      </c>
+      <c r="H245">
         <f t="shared" si="9"/>
-        <v>10.973583186934738</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A245" s="5" t="s">
-        <v>25</v>
+        <v>6.0390396252195968</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B246">
-        <v>2.0895428260830022</v>
+        <v>1.7682399234246267</v>
       </c>
       <c r="C246">
-        <v>6.0390396252195968</v>
+        <v>4.4197410371527095</v>
       </c>
       <c r="E246" t="s">
         <v>274</v>
@@ -13783,22 +13784,22 @@
       </c>
       <c r="G246">
         <f t="shared" si="8"/>
-        <v>2.0895428260830022</v>
+        <v>1.7682399234246267</v>
       </c>
       <c r="H246">
         <f t="shared" si="9"/>
-        <v>6.0390396252195968</v>
+        <v>4.4197410371527095</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B247">
-        <v>1.7682399234246267</v>
+        <v>1.7605305508181868</v>
       </c>
       <c r="C247">
-        <v>4.4197410371527095</v>
+        <v>4.8755937276335475</v>
       </c>
       <c r="E247" t="s">
         <v>274</v>
@@ -13808,22 +13809,22 @@
       </c>
       <c r="G247">
         <f t="shared" si="8"/>
-        <v>1.7682399234246267</v>
+        <v>1.7605305508181868</v>
       </c>
       <c r="H247">
         <f t="shared" si="9"/>
-        <v>4.4197410371527095</v>
+        <v>4.8755937276335475</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B248">
-        <v>1.7605305508181868</v>
+        <v>0.6710786851257553</v>
       </c>
       <c r="C248">
-        <v>4.8755937276335475</v>
+        <v>1.3043789446287981</v>
       </c>
       <c r="E248" t="s">
         <v>274</v>
@@ -13833,22 +13834,22 @@
       </c>
       <c r="G248">
         <f t="shared" si="8"/>
-        <v>1.7605305508181868</v>
+        <v>0.6710786851257553</v>
       </c>
       <c r="H248">
         <f t="shared" si="9"/>
-        <v>4.8755937276335475</v>
+        <v>1.3043789446287981</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B249">
-        <v>0.6710786851257553</v>
+        <v>1.8357228345518393</v>
       </c>
       <c r="C249">
-        <v>1.3043789446287981</v>
+        <v>3.923417268527555</v>
       </c>
       <c r="E249" t="s">
         <v>274</v>
@@ -13858,22 +13859,22 @@
       </c>
       <c r="G249">
         <f t="shared" si="8"/>
-        <v>0.6710786851257553</v>
+        <v>1.8357228345518393</v>
       </c>
       <c r="H249">
         <f t="shared" si="9"/>
-        <v>1.3043789446287981</v>
+        <v>3.923417268527555</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B250">
-        <v>1.8357228345518393</v>
+        <v>2.4473727955220608</v>
       </c>
       <c r="C250">
-        <v>3.923417268527555</v>
+        <v>5.0871234302817356</v>
       </c>
       <c r="E250" t="s">
         <v>274</v>
@@ -13883,22 +13884,22 @@
       </c>
       <c r="G250">
         <f t="shared" si="8"/>
-        <v>1.8357228345518393</v>
+        <v>2.4473727955220608</v>
       </c>
       <c r="H250">
         <f t="shared" si="9"/>
-        <v>3.923417268527555</v>
+        <v>5.0871234302817356</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B251">
-        <v>2.4473727955220608</v>
+        <v>1.4663977535465109</v>
       </c>
       <c r="C251">
-        <v>5.0871234302817356</v>
+        <v>4.0234888411737906</v>
       </c>
       <c r="E251" t="s">
         <v>274</v>
@@ -13908,22 +13909,22 @@
       </c>
       <c r="G251">
         <f t="shared" si="8"/>
-        <v>2.4473727955220608</v>
+        <v>1.4663977535465109</v>
       </c>
       <c r="H251">
         <f t="shared" si="9"/>
-        <v>5.0871234302817356</v>
+        <v>4.0234888411737906</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B252">
-        <v>1.4663977535465109</v>
+        <v>1.40466800842395</v>
       </c>
       <c r="C252">
-        <v>4.0234888411737906</v>
+        <v>3.3887045351031295</v>
       </c>
       <c r="E252" t="s">
         <v>274</v>
@@ -13933,22 +13934,22 @@
       </c>
       <c r="G252">
         <f t="shared" si="8"/>
-        <v>1.4663977535465109</v>
+        <v>1.40466800842395</v>
       </c>
       <c r="H252">
         <f t="shared" si="9"/>
-        <v>4.0234888411737906</v>
+        <v>3.3887045351031295</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B253">
-        <v>1.40466800842395</v>
+        <v>2.5026376835506938</v>
       </c>
       <c r="C253">
-        <v>3.3887045351031295</v>
+        <v>6.4176589238076636</v>
       </c>
       <c r="E253" t="s">
         <v>274</v>
@@ -13958,22 +13959,22 @@
       </c>
       <c r="G253">
         <f t="shared" si="8"/>
-        <v>1.40466800842395</v>
+        <v>2.5026376835506938</v>
       </c>
       <c r="H253">
         <f t="shared" si="9"/>
-        <v>3.3887045351031295</v>
+        <v>6.4176589238076636</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B254">
-        <v>2.5026376835506938</v>
+        <v>0.62102225203959105</v>
       </c>
       <c r="C254">
-        <v>6.4176589238076636</v>
+        <v>1.3374324939813909</v>
       </c>
       <c r="E254" t="s">
         <v>274</v>
@@ -13983,22 +13984,22 @@
       </c>
       <c r="G254">
         <f t="shared" si="8"/>
-        <v>2.5026376835506938</v>
+        <v>0.62102225203959105</v>
       </c>
       <c r="H254">
         <f t="shared" si="9"/>
-        <v>6.4176589238076636</v>
+        <v>1.3374324939813909</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B255">
-        <v>0.62102225203959105</v>
+        <v>1.6964212383095882</v>
       </c>
       <c r="C255">
-        <v>1.3374324939813909</v>
+        <v>3.7748714945669848</v>
       </c>
       <c r="E255" t="s">
         <v>274</v>
@@ -14008,22 +14009,22 @@
       </c>
       <c r="G255">
         <f t="shared" si="8"/>
-        <v>0.62102225203959105</v>
+        <v>1.6964212383095882</v>
       </c>
       <c r="H255">
         <f t="shared" si="9"/>
-        <v>1.3374324939813909</v>
+        <v>3.7748714945669848</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B256">
-        <v>1.6964212383095882</v>
+        <v>1.9166854498254555</v>
       </c>
       <c r="C256">
-        <v>3.7748714945669848</v>
+        <v>4.5460992907801412</v>
       </c>
       <c r="E256" t="s">
         <v>274</v>
@@ -14033,22 +14034,22 @@
       </c>
       <c r="G256">
         <f t="shared" si="8"/>
-        <v>1.6964212383095882</v>
+        <v>1.9166854498254555</v>
       </c>
       <c r="H256">
         <f t="shared" si="9"/>
-        <v>3.7748714945669848</v>
+        <v>4.5460992907801412</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B257">
-        <v>1.9166854498254555</v>
+        <v>1.6953172201409299</v>
       </c>
       <c r="C257">
-        <v>4.5460992907801412</v>
+        <v>3.8806688789120947</v>
       </c>
       <c r="E257" t="s">
         <v>274</v>
@@ -14058,22 +14059,22 @@
       </c>
       <c r="G257">
         <f t="shared" si="8"/>
-        <v>1.9166854498254555</v>
+        <v>1.6953172201409299</v>
       </c>
       <c r="H257">
         <f t="shared" si="9"/>
-        <v>4.5460992907801412</v>
+        <v>3.8806688789120947</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B258">
-        <v>1.6953172201409299</v>
+        <v>1.6030611180612686</v>
       </c>
       <c r="C258">
-        <v>3.8806688789120947</v>
+        <v>2.7643307957576937</v>
       </c>
       <c r="E258" t="s">
         <v>274</v>
@@ -14083,22 +14084,22 @@
       </c>
       <c r="G258">
         <f t="shared" si="8"/>
-        <v>1.6953172201409299</v>
+        <v>1.6030611180612686</v>
       </c>
       <c r="H258">
         <f t="shared" si="9"/>
-        <v>3.8806688789120947</v>
+        <v>2.7643307957576937</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B259">
-        <v>1.6030611180612686</v>
+        <v>2.0822836491184824</v>
       </c>
       <c r="C259">
-        <v>2.7643307957576937</v>
+        <v>4.8396772724315174</v>
       </c>
       <c r="E259" t="s">
         <v>274</v>
@@ -14108,22 +14109,22 @@
       </c>
       <c r="G259">
         <f t="shared" si="8"/>
-        <v>1.6030611180612686</v>
+        <v>2.0822836491184824</v>
       </c>
       <c r="H259">
         <f t="shared" si="9"/>
-        <v>2.7643307957576937</v>
+        <v>4.8396772724315174</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B260">
-        <v>2.0822836491184824</v>
+        <v>1.582139578382648</v>
       </c>
       <c r="C260">
-        <v>4.8396772724315174</v>
+        <v>3.3006701802329359</v>
       </c>
       <c r="E260" t="s">
         <v>274</v>
@@ -14133,22 +14134,22 @@
       </c>
       <c r="G260">
         <f t="shared" si="8"/>
-        <v>2.0822836491184824</v>
+        <v>1.582139578382648</v>
       </c>
       <c r="H260">
         <f t="shared" si="9"/>
-        <v>4.8396772724315174</v>
+        <v>3.3006701802329359</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B261">
-        <v>1.582139578382648</v>
+        <v>0.83148200076518108</v>
       </c>
       <c r="C261">
-        <v>3.3006701802329359</v>
+        <v>1.6349795041967594</v>
       </c>
       <c r="E261" t="s">
         <v>274</v>
@@ -14158,22 +14159,22 @@
       </c>
       <c r="G261">
         <f t="shared" si="8"/>
-        <v>1.582139578382648</v>
+        <v>0.83148200076518108</v>
       </c>
       <c r="H261">
         <f t="shared" si="9"/>
-        <v>3.3006701802329359</v>
+        <v>1.6349795041967594</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B262">
-        <v>0.83148200076518108</v>
+        <v>2.3747249115442881</v>
       </c>
       <c r="C262">
-        <v>1.6349795041967594</v>
+        <v>5.1261630555013333</v>
       </c>
       <c r="E262" t="s">
         <v>274</v>
@@ -14183,22 +14184,22 @@
       </c>
       <c r="G262">
         <f t="shared" si="8"/>
-        <v>0.83148200076518108</v>
+        <v>2.3747249115442881</v>
       </c>
       <c r="H262">
         <f t="shared" si="9"/>
-        <v>1.6349795041967594</v>
+        <v>5.1261630555013333</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B263">
-        <v>2.3747249115442881</v>
+        <v>2.4217420827124001</v>
       </c>
       <c r="C263">
-        <v>5.1261630555013333</v>
+        <v>5.7035591124991862</v>
       </c>
       <c r="E263" t="s">
         <v>274</v>
@@ -14208,22 +14209,22 @@
       </c>
       <c r="G263">
         <f t="shared" si="8"/>
-        <v>2.3747249115442881</v>
+        <v>2.4217420827124001</v>
       </c>
       <c r="H263">
         <f t="shared" si="9"/>
-        <v>5.1261630555013333</v>
+        <v>5.7035591124991862</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A264" s="3" t="s">
-        <v>251</v>
+      <c r="A264" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B264">
-        <v>2.4217420827124001</v>
+        <v>2.3356728507574438</v>
       </c>
       <c r="C264">
-        <v>5.7035591124991862</v>
+        <v>5.6222265599583574</v>
       </c>
       <c r="E264" t="s">
         <v>274</v>
@@ -14233,22 +14234,22 @@
       </c>
       <c r="G264">
         <f t="shared" si="8"/>
-        <v>2.4217420827124001</v>
+        <v>2.3356728507574438</v>
       </c>
       <c r="H264">
         <f t="shared" si="9"/>
-        <v>5.7035591124991862</v>
+        <v>5.6222265599583574</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B265">
-        <v>2.3356728507574438</v>
+        <v>2.3323450889041832</v>
       </c>
       <c r="C265">
-        <v>5.6222265599583574</v>
+        <v>6.1446418114386088</v>
       </c>
       <c r="E265" t="s">
         <v>274</v>
@@ -14258,22 +14259,22 @@
       </c>
       <c r="G265">
         <f t="shared" si="8"/>
-        <v>2.3356728507574438</v>
+        <v>2.3323450889041832</v>
       </c>
       <c r="H265">
         <f t="shared" si="9"/>
-        <v>5.6222265599583574</v>
+        <v>6.1446418114386088</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B266">
-        <v>2.3323450889041832</v>
+        <v>2.02635738649685</v>
       </c>
       <c r="C266">
-        <v>6.1446418114386088</v>
+        <v>4.5001626651050808</v>
       </c>
       <c r="E266" t="s">
         <v>274</v>
@@ -14283,22 +14284,22 @@
       </c>
       <c r="G266">
         <f t="shared" si="8"/>
-        <v>2.3323450889041832</v>
+        <v>2.02635738649685</v>
       </c>
       <c r="H266">
         <f t="shared" si="9"/>
-        <v>6.1446418114386088</v>
+        <v>4.5001626651050808</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B267">
-        <v>2.02635738649685</v>
+        <v>1.0319389506961829</v>
       </c>
       <c r="C267">
-        <v>4.5001626651050808</v>
+        <v>1.6877480642852491</v>
       </c>
       <c r="E267" t="s">
         <v>274</v>
@@ -14308,22 +14309,22 @@
       </c>
       <c r="G267">
         <f t="shared" si="8"/>
-        <v>2.02635738649685</v>
+        <v>1.0319389506961829</v>
       </c>
       <c r="H267">
         <f t="shared" si="9"/>
-        <v>4.5001626651050808</v>
+        <v>1.6877480642852491</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B268">
-        <v>1.0319389506961829</v>
+        <v>1.5020685065156065</v>
       </c>
       <c r="C268">
-        <v>1.6877480642852491</v>
+        <v>2.1458780662372305</v>
       </c>
       <c r="E268" t="s">
         <v>274</v>
@@ -14333,61 +14334,36 @@
       </c>
       <c r="G268">
         <f t="shared" si="8"/>
-        <v>1.0319389506961829</v>
+        <v>1.5020685065156065</v>
       </c>
       <c r="H268">
         <f t="shared" si="9"/>
-        <v>1.6877480642852491</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A269" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B269">
-        <v>1.5020685065156065</v>
-      </c>
-      <c r="C269">
         <v>2.1458780662372305</v>
       </c>
-      <c r="E269" t="s">
-        <v>274</v>
-      </c>
-      <c r="F269" t="s">
-        <v>19</v>
-      </c>
-      <c r="G269">
-        <f t="shared" si="8"/>
-        <v>1.5020685065156065</v>
-      </c>
-      <c r="H269">
-        <f t="shared" si="9"/>
-        <v>2.1458780662372305</v>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A270" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B270">
+        <f>MAX(B2:B268)</f>
+        <v>19.4665</v>
+      </c>
+      <c r="C270">
+        <f>MAX(C2:C268)</f>
+        <v>13.523716572320904</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B271">
-        <f>MAX(B2:B269)</f>
-        <v>19.4665</v>
+        <f>MIN(B2:B268)</f>
+        <v>0.19661639553720142</v>
       </c>
       <c r="C271">
-        <f>MAX(C2:C269)</f>
-        <v>13.523716572320904</v>
-      </c>
-    </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A272" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B272">
-        <f>MIN(B2:B269)</f>
-        <v>0.19661639553720142</v>
-      </c>
-      <c r="C272">
-        <f>MIN(C2:C269)</f>
+        <f>MIN(C2:C268)</f>
         <v>1.6352156002086744E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add J088 data from Yuanyuan
</commit_message>
<xml_diff>
--- a/CL Brightness DUvsDTh mol%.xlsx
+++ b/CL Brightness DUvsDTh mol%.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n733m382/Documents/GitHub/DUDThZircon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39561364-1AD6-4845-97C1-2ED5B6C27B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93CF33D-C417-024F-B7E0-76DB260CBAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1300" windowWidth="28180" windowHeight="27500" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
+    <workbookView xWindow="20000" yWindow="1240" windowWidth="28180" windowHeight="27500" activeTab="1" xr2:uid="{155AF1BA-5B7E-6A43-9689-19AAEAC8D4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="276">
   <si>
     <t>DARK</t>
   </si>
@@ -862,6 +862,9 @@
   </si>
   <si>
     <t>H091</t>
+  </si>
+  <si>
+    <t>J088</t>
   </si>
 </sst>
 </file>
@@ -5126,8 +5129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49F7A8F-203D-5E4B-98FB-041431663A31}">
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView topLeftCell="B86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="A244" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8042,10 +8045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F37500E-3173-B64C-94B9-2EBED4B5FAA5}">
-  <dimension ref="A1:H271"/>
+  <dimension ref="A1:H288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178:XFD178"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A290" sqref="A290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14341,30 +14344,471 @@
         <v>2.1458780662372305</v>
       </c>
     </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" t="s">
+        <v>17</v>
+      </c>
+      <c r="C269" t="s">
+        <v>18</v>
+      </c>
+      <c r="E269" s="2"/>
+    </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="B270">
-        <f>MAX(B2:B268)</f>
-        <v>19.4665</v>
+        <v>7.6044379255531567</v>
       </c>
       <c r="C270">
-        <f>MAX(C2:C268)</f>
-        <v>13.523716572320904</v>
+        <v>4.9940033636871544</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F270" t="s">
+        <v>100</v>
+      </c>
+      <c r="G270">
+        <f>B270</f>
+        <v>7.6044379255531567</v>
+      </c>
+      <c r="H270">
+        <f>C270</f>
+        <v>4.9940033636871544</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="B271">
-        <f>MIN(B2:B268)</f>
-        <v>0.19661639553720142</v>
+        <v>7.449855047858768</v>
       </c>
       <c r="C271">
-        <f>MIN(C2:C268)</f>
-        <v>1.6352156002086744E-2</v>
+        <v>4.982827504310813</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F271" t="s">
+        <v>100</v>
+      </c>
+      <c r="G271">
+        <f t="shared" ref="G271:G278" si="10">B271</f>
+        <v>7.449855047858768</v>
+      </c>
+      <c r="H271">
+        <f t="shared" ref="H271:H278" si="11">C271</f>
+        <v>4.982827504310813</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A272" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B272">
+        <v>4.9805936583139614</v>
+      </c>
+      <c r="C272">
+        <v>3.0603781441021165</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F272" t="s">
+        <v>100</v>
+      </c>
+      <c r="G272">
+        <f t="shared" si="10"/>
+        <v>4.9805936583139614</v>
+      </c>
+      <c r="H272">
+        <f t="shared" si="11"/>
+        <v>3.0603781441021165</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A273" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B273">
+        <v>4.2841936663886031</v>
+      </c>
+      <c r="C273">
+        <v>2.7233242815024612</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F273" t="s">
+        <v>100</v>
+      </c>
+      <c r="G273">
+        <f t="shared" si="10"/>
+        <v>4.2841936663886031</v>
+      </c>
+      <c r="H273">
+        <f t="shared" si="11"/>
+        <v>2.7233242815024612</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A274" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B274">
+        <v>4.916394520179284</v>
+      </c>
+      <c r="C274">
+        <v>2.8869535542142217</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F274" t="s">
+        <v>100</v>
+      </c>
+      <c r="G274">
+        <f t="shared" si="10"/>
+        <v>4.916394520179284</v>
+      </c>
+      <c r="H274">
+        <f t="shared" si="11"/>
+        <v>2.8869535542142217</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A275" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B275">
+        <v>4.4334132875956591</v>
+      </c>
+      <c r="C275">
+        <v>2.7964247085539609</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F275" t="s">
+        <v>100</v>
+      </c>
+      <c r="G275">
+        <f t="shared" si="10"/>
+        <v>4.4334132875956591</v>
+      </c>
+      <c r="H275">
+        <f t="shared" si="11"/>
+        <v>2.7964247085539609</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A276" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B276">
+        <v>4.9307824446764785</v>
+      </c>
+      <c r="C276">
+        <v>3.4224743164471358</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F276" t="s">
+        <v>100</v>
+      </c>
+      <c r="G276">
+        <f t="shared" si="10"/>
+        <v>4.9307824446764785</v>
+      </c>
+      <c r="H276">
+        <f t="shared" si="11"/>
+        <v>3.4224743164471358</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A277" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B277">
+        <v>4.7188352588500786</v>
+      </c>
+      <c r="C277">
+        <v>3.241562268525974</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F277" t="s">
+        <v>100</v>
+      </c>
+      <c r="G277">
+        <f t="shared" si="10"/>
+        <v>4.7188352588500786</v>
+      </c>
+      <c r="H277">
+        <f t="shared" si="11"/>
+        <v>3.241562268525974</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A278" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B278">
+        <v>4.7880528141735992</v>
+      </c>
+      <c r="C278">
+        <v>3.0574297124086187</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F278" t="s">
+        <v>100</v>
+      </c>
+      <c r="G278">
+        <f t="shared" si="10"/>
+        <v>4.7880528141735992</v>
+      </c>
+      <c r="H278">
+        <f t="shared" si="11"/>
+        <v>3.0574297124086187</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A280" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B280">
+        <v>3.049237015043655</v>
+      </c>
+      <c r="C280">
+        <v>1.5495900311668434</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F280" t="s">
+        <v>19</v>
+      </c>
+      <c r="G280">
+        <f>B280</f>
+        <v>3.049237015043655</v>
+      </c>
+      <c r="H280">
+        <f>C280</f>
+        <v>1.5495900311668434</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A281" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B281">
+        <v>2.9926175205895444</v>
+      </c>
+      <c r="C281">
+        <v>1.3909776813414279</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F281" t="s">
+        <v>19</v>
+      </c>
+      <c r="G281">
+        <f t="shared" ref="G281:G288" si="12">B281</f>
+        <v>2.9926175205895444</v>
+      </c>
+      <c r="H281">
+        <f t="shared" ref="H281:H288" si="13">C281</f>
+        <v>1.3909776813414279</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A282" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B282">
+        <v>3.5940546942409966</v>
+      </c>
+      <c r="C282">
+        <v>1.6952622648727274</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F282" t="s">
+        <v>19</v>
+      </c>
+      <c r="G282">
+        <f t="shared" si="12"/>
+        <v>3.5940546942409966</v>
+      </c>
+      <c r="H282">
+        <f t="shared" si="13"/>
+        <v>1.6952622648727274</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A283" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B283">
+        <v>4.4072763009402971</v>
+      </c>
+      <c r="C283">
+        <v>2.2108643053011772</v>
+      </c>
+      <c r="E283" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F283" t="s">
+        <v>19</v>
+      </c>
+      <c r="G283">
+        <f t="shared" si="12"/>
+        <v>4.4072763009402971</v>
+      </c>
+      <c r="H283">
+        <f t="shared" si="13"/>
+        <v>2.2108643053011772</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B284">
+        <v>0.3496203140788654</v>
+      </c>
+      <c r="C284">
+        <v>0.17164864874609742</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F284" t="s">
+        <v>19</v>
+      </c>
+      <c r="G284">
+        <f t="shared" si="12"/>
+        <v>0.3496203140788654</v>
+      </c>
+      <c r="H284">
+        <f t="shared" si="13"/>
+        <v>0.17164864874609742</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A285" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B285">
+        <v>0.38976938956873225</v>
+      </c>
+      <c r="C285">
+        <v>0.19281644344871815</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F285" t="s">
+        <v>19</v>
+      </c>
+      <c r="G285">
+        <f t="shared" si="12"/>
+        <v>0.38976938956873225</v>
+      </c>
+      <c r="H285">
+        <f t="shared" si="13"/>
+        <v>0.19281644344871815</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A286" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B286">
+        <v>2.9094257140474036</v>
+      </c>
+      <c r="C286">
+        <v>1.4459182047490011</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F286" t="s">
+        <v>19</v>
+      </c>
+      <c r="G286">
+        <f t="shared" si="12"/>
+        <v>2.9094257140474036</v>
+      </c>
+      <c r="H286">
+        <f t="shared" si="13"/>
+        <v>1.4459182047490011</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A287" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B287">
+        <v>2.5072417393647477</v>
+      </c>
+      <c r="C287">
+        <v>1.0653441113007633</v>
+      </c>
+      <c r="E287" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F287" t="s">
+        <v>19</v>
+      </c>
+      <c r="G287">
+        <f t="shared" si="12"/>
+        <v>2.5072417393647477</v>
+      </c>
+      <c r="H287">
+        <f t="shared" si="13"/>
+        <v>1.0653441113007633</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A288" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B288">
+        <v>2.6561184277004948</v>
+      </c>
+      <c r="C288">
+        <v>0.98700524942835999</v>
+      </c>
+      <c r="E288" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F288" t="s">
+        <v>19</v>
+      </c>
+      <c r="G288">
+        <f t="shared" si="12"/>
+        <v>2.6561184277004948</v>
+      </c>
+      <c r="H288">
+        <f t="shared" si="13"/>
+        <v>0.98700524942835999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>